<commit_message>
backend - 1# refactor on excel(remove gap), 2# added method equals product, only by name and unit, 3# now shopping list return product without repeat
</commit_message>
<xml_diff>
--- a/BackEnd/ExcelReader/src/main/resources/data/jadlospis2.xlsx
+++ b/BackEnd/ExcelReader/src/main/resources/data/jadlospis2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMOWANIE\etmeall2\EatMeAll\ExcelReader\src\main\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMOWANIE\etmeall2\EatMeAll\BackEnd\ExcelReader\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D214D77-EA08-41C6-97F1-852050855528}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ADCC25-0059-4C3E-AA02-73A504309C0A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{DC9E3696-05CD-4AC0-85C8-C796492A84E0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="156">
   <si>
     <t>Koktajl mleczny z otrębami</t>
   </si>
@@ -120,9 +120,6 @@
     <t>2 łyzki</t>
   </si>
   <si>
-    <t xml:space="preserve">jogurt naturalny </t>
-  </si>
-  <si>
     <t>1/2 opako.</t>
   </si>
   <si>
@@ -174,18 +171,12 @@
     <t>Do przegryzania: wafle ryżowe słodkie ulubiony rodzaj (np. w polewie jogurtowej, 2 szt).</t>
   </si>
   <si>
-    <t xml:space="preserve">masło </t>
-  </si>
-  <si>
     <t>1/2 łyzeczki</t>
   </si>
   <si>
     <t>1 plasterek</t>
   </si>
   <si>
-    <t xml:space="preserve">sałata </t>
-  </si>
-  <si>
     <t>1 liść</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>1 plaster</t>
   </si>
   <si>
-    <t>sałata,</t>
-  </si>
-  <si>
     <t>1 lisc</t>
   </si>
   <si>
@@ -303,9 +291,6 @@
     <t>Roladki schabowe z ziemniakami z pietruszką, Surówka ulubiona</t>
   </si>
   <si>
-    <t>Schab bez kości</t>
-  </si>
-  <si>
     <t>ser żółty</t>
   </si>
   <si>
@@ -339,9 +324,6 @@
     <t xml:space="preserve">Wymieszać twarożek ze szczypiorkiem i solą; kanapki przygotować z serkiem </t>
   </si>
   <si>
-    <t>maslo</t>
-  </si>
-  <si>
     <t>1/2 lyzeczki</t>
   </si>
   <si>
@@ -372,15 +354,9 @@
     <t>2 plastry</t>
   </si>
   <si>
-    <t>ser zółty,</t>
-  </si>
-  <si>
     <t>1 cienki plaster</t>
   </si>
   <si>
-    <t xml:space="preserve">keczup </t>
-  </si>
-  <si>
     <t>Papryka faszerowana</t>
   </si>
   <si>
@@ -462,12 +438,6 @@
     <t>jeżyny</t>
   </si>
   <si>
-    <t xml:space="preserve">bułkę kajzerkę </t>
-  </si>
-  <si>
-    <t xml:space="preserve">jajko </t>
-  </si>
-  <si>
     <t>chleb żytni razowy</t>
   </si>
   <si>
@@ -504,13 +474,25 @@
     <t>bułka do hamburgerów</t>
   </si>
   <si>
-    <t xml:space="preserve">ziemniaki </t>
-  </si>
-  <si>
     <t>surówka gotowa</t>
   </si>
   <si>
-    <t xml:space="preserve">ryż </t>
+    <t>ser zółty</t>
+  </si>
+  <si>
+    <t>schab bez kości</t>
+  </si>
+  <si>
+    <t>bułka kajzerka</t>
+  </si>
+  <si>
+    <t>ziemniaki</t>
+  </si>
+  <si>
+    <t>keczup</t>
+  </si>
+  <si>
+    <t>ryż</t>
   </si>
 </sst>
 </file>
@@ -890,13 +872,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1838D449-8DD4-4711-984B-E0AC88629B5C}">
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="43.77734375" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" customWidth="1"/>
     <col min="9" max="9" width="78.77734375" customWidth="1"/>
   </cols>
@@ -906,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1">
         <v>10</v>
@@ -915,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F1" s="1">
         <v>400</v>
@@ -963,7 +946,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F3" s="1">
         <v>100</v>
@@ -984,7 +967,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F4" s="1">
         <v>200</v>
@@ -1005,7 +988,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1019,7 +1002,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C6" s="1">
         <v>10</v>
@@ -1028,7 +1011,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F6" s="1">
         <v>200</v>
@@ -1118,7 +1101,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1132,7 +1115,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C11" s="1">
         <v>10</v>
@@ -1141,7 +1124,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F11" s="1">
         <v>200</v>
@@ -1231,7 +1214,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1245,7 +1228,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C16" s="1">
         <v>20</v>
@@ -1254,7 +1237,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="F16" s="1">
         <v>100</v>
@@ -1266,7 +1249,7 @@
         <v>21</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="J16" s="1">
         <v>300</v>
@@ -1281,7 +1264,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F17" s="1">
         <v>120</v>
@@ -1342,7 +1325,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F20" s="1">
         <v>75</v>
@@ -1363,7 +1346,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1377,7 +1360,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C22" s="1">
         <v>20</v>
@@ -1398,7 +1381,7 @@
         <v>29</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="J22" s="1">
         <v>300</v>
@@ -1413,7 +1396,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F23" s="1">
         <v>30</v>
@@ -1434,7 +1417,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="F24" s="1">
         <v>80</v>
@@ -1443,7 +1426,7 @@
         <v>6</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1455,7 +1438,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F25" s="1">
         <v>30</v>
@@ -1464,7 +1447,7 @@
         <v>6</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1476,7 +1459,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F26" s="1">
         <v>20</v>
@@ -1485,7 +1468,7 @@
         <v>6</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1497,7 +1480,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F27" s="1">
         <v>12</v>
@@ -1506,7 +1489,7 @@
         <v>6</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1518,7 +1501,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1532,16 +1515,16 @@
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C29" s="1">
         <v>30</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="F29" s="1">
         <v>75</v>
@@ -1550,10 +1533,10 @@
         <v>6</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="J29" s="1">
         <v>300</v>
@@ -1568,7 +1551,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="F30" s="1">
         <v>80</v>
@@ -1577,7 +1560,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -1589,7 +1572,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F31" s="1">
         <v>100</v>
@@ -1598,7 +1581,7 @@
         <v>6</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1610,7 +1593,7 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F32" s="1">
         <v>100</v>
@@ -1619,7 +1602,7 @@
         <v>6</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1631,7 +1614,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1645,16 +1628,16 @@
         <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C34" s="1">
         <v>15</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F34" s="1">
         <v>50</v>
@@ -1663,10 +1646,10 @@
         <v>6</v>
       </c>
       <c r="H34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="J34" s="1">
         <v>350</v>
@@ -1681,7 +1664,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="F35" s="1">
         <v>5</v>
@@ -1690,7 +1673,7 @@
         <v>6</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1711,7 +1694,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -1723,7 +1706,7 @@
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="F37" s="1">
         <v>15</v>
@@ -1732,7 +1715,7 @@
         <v>6</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -1744,7 +1727,7 @@
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F38" s="1">
         <v>20</v>
@@ -1753,7 +1736,7 @@
         <v>6</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -1765,7 +1748,7 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F39" s="1">
         <v>150</v>
@@ -1774,7 +1757,7 @@
         <v>6</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -1786,7 +1769,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1800,16 +1783,16 @@
         <v>8</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C41" s="1">
         <v>15</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F41" s="1">
         <v>160</v>
@@ -1818,10 +1801,10 @@
         <v>6</v>
       </c>
       <c r="H41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="J41" s="1">
         <v>350</v>
@@ -1836,7 +1819,7 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F42" s="1">
         <v>30</v>
@@ -1845,7 +1828,7 @@
         <v>6</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -1857,7 +1840,7 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -1871,16 +1854,16 @@
         <v>9</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C44" s="1">
         <v>15</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="F44" s="1">
         <v>80</v>
@@ -1889,10 +1872,10 @@
         <v>6</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J44" s="1">
         <v>350</v>
@@ -1916,7 +1899,7 @@
         <v>6</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -1928,7 +1911,7 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F46" s="1">
         <v>20</v>
@@ -1937,7 +1920,7 @@
         <v>6</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -1949,7 +1932,7 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F47" s="1">
         <v>10</v>
@@ -1958,7 +1941,7 @@
         <v>6</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -1970,7 +1953,7 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F48" s="1">
         <v>50</v>
@@ -1979,7 +1962,7 @@
         <v>6</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -1991,7 +1974,7 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2005,16 +1988,16 @@
         <v>10</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C50" s="1">
         <v>30</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F50" s="1">
         <v>200</v>
@@ -2023,16 +2006,16 @@
         <v>6</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="J50" s="1">
         <v>300</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2041,7 +2024,7 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F51" s="1">
         <v>500</v>
@@ -2050,7 +2033,7 @@
         <v>6</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -2062,7 +2045,7 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -2076,16 +2059,16 @@
         <v>11</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C53" s="1">
         <v>30</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F53" s="1">
         <v>200</v>
@@ -2094,16 +2077,16 @@
         <v>6</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="J53" s="1">
         <v>300</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2112,7 +2095,7 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F54" s="1">
         <v>500</v>
@@ -2121,7 +2104,7 @@
         <v>6</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
@@ -2133,7 +2116,7 @@
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -2147,16 +2130,16 @@
         <v>12</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C56" s="1">
         <v>30</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F56" s="1">
         <v>200</v>
@@ -2165,16 +2148,16 @@
         <v>6</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="J56" s="1">
         <v>300</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2183,7 +2166,7 @@
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -2197,16 +2180,16 @@
         <v>13</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C58" s="1">
         <v>45</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F58" s="1">
         <v>150</v>
@@ -2215,10 +2198,10 @@
         <v>6</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="J58" s="1">
         <v>600</v>
@@ -2233,7 +2216,7 @@
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F59" s="1">
         <v>150</v>
@@ -2242,7 +2225,7 @@
         <v>6</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
@@ -2254,7 +2237,7 @@
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="F60" s="1">
         <v>5</v>
@@ -2263,7 +2246,7 @@
         <v>6</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
@@ -2275,7 +2258,7 @@
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="F61" s="1">
         <v>200</v>
@@ -2284,7 +2267,7 @@
         <v>6</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
@@ -2296,7 +2279,7 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F62" s="1">
         <v>200</v>
@@ -2305,7 +2288,7 @@
         <v>6</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -2317,7 +2300,7 @@
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F63" s="1">
         <v>75</v>
@@ -2326,7 +2309,7 @@
         <v>6</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
@@ -2338,7 +2321,7 @@
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F64" s="1">
         <v>75</v>
@@ -2347,7 +2330,7 @@
         <v>6</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
@@ -2359,7 +2342,7 @@
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -2373,16 +2356,16 @@
         <v>14</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C66" s="1">
         <v>45</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F66" s="1">
         <v>150</v>
@@ -2391,10 +2374,10 @@
         <v>6</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="J66" s="1">
         <v>600</v>
@@ -2409,7 +2392,7 @@
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="F67" s="1">
         <v>5</v>
@@ -2418,7 +2401,7 @@
         <v>6</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
@@ -2430,7 +2413,7 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="F68" s="1">
         <v>55</v>
@@ -2439,7 +2422,7 @@
         <v>6</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
@@ -2451,7 +2434,7 @@
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F69" s="1">
         <v>8</v>
@@ -2460,7 +2443,7 @@
         <v>6</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
@@ -2472,7 +2455,7 @@
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F70" s="1">
         <v>40</v>
@@ -2493,7 +2476,7 @@
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F71" s="1">
         <v>5</v>
@@ -2502,7 +2485,7 @@
         <v>6</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
@@ -2514,7 +2497,7 @@
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F72" s="1">
         <v>8</v>
@@ -2523,7 +2506,7 @@
         <v>6</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
@@ -2535,7 +2518,7 @@
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F73" s="1">
         <v>15</v>
@@ -2544,7 +2527,7 @@
         <v>6</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
@@ -2556,7 +2539,7 @@
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F74" s="1">
         <v>5</v>
@@ -2565,7 +2548,7 @@
         <v>6</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
@@ -2577,7 +2560,7 @@
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F75" s="1">
         <v>75</v>
@@ -2596,7 +2579,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F76" s="1">
         <v>30</v>
@@ -2605,7 +2588,7 @@
         <v>6</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
@@ -2617,7 +2600,7 @@
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F77" s="1">
         <v>75</v>
@@ -2626,7 +2609,7 @@
         <v>6</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
@@ -2638,7 +2621,7 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F78" s="1">
         <v>20</v>
@@ -2647,7 +2630,7 @@
         <v>6</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
@@ -2659,7 +2642,7 @@
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -2673,16 +2656,16 @@
         <v>15</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C80" s="1">
         <v>45</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="F80" s="1">
         <v>100</v>
@@ -2691,10 +2674,10 @@
         <v>6</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="J80" s="1">
         <v>600</v>
@@ -2709,7 +2692,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F81" s="1">
         <v>10</v>
@@ -2718,7 +2701,7 @@
         <v>6</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
@@ -2730,7 +2713,7 @@
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F82" s="1">
         <v>30</v>
@@ -2739,7 +2722,7 @@
         <v>6</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
@@ -2751,7 +2734,7 @@
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F83" s="1">
         <v>30</v>
@@ -2760,7 +2743,7 @@
         <v>6</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
@@ -2772,7 +2755,7 @@
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F84" s="1">
         <v>200</v>
@@ -2781,7 +2764,7 @@
         <v>6</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
@@ -2793,7 +2776,7 @@
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F85" s="1">
         <v>40</v>
@@ -2802,7 +2785,7 @@
         <v>6</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
@@ -2814,7 +2797,7 @@
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="F86" s="1">
         <v>100</v>
@@ -2823,7 +2806,7 @@
         <v>6</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
@@ -2835,7 +2818,7 @@
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F87" s="1">
         <v>200</v>
@@ -2844,7 +2827,7 @@
         <v>1</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
@@ -2856,7 +2839,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -2870,16 +2853,16 @@
         <v>16</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C89" s="1">
         <v>10</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F89" s="1">
         <v>80</v>
@@ -2888,10 +2871,10 @@
         <v>6</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J89" s="1">
         <v>350</v>
@@ -2906,7 +2889,7 @@
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="F90" s="1">
         <v>5</v>
@@ -2915,10 +2898,10 @@
         <v>6</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
@@ -2929,7 +2912,7 @@
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F91" s="1">
         <v>50</v>
@@ -2950,7 +2933,7 @@
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F92" s="1">
         <v>30</v>
@@ -2971,7 +2954,7 @@
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F93" s="1">
         <v>50</v>
@@ -3001,7 +2984,7 @@
         <v>6</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
@@ -3013,7 +2996,7 @@
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F95" s="1">
         <v>100</v>
@@ -3022,7 +3005,7 @@
         <v>6</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
@@ -3034,7 +3017,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
@@ -3048,16 +3031,16 @@
         <v>17</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C97" s="1">
         <v>10</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F97" s="1">
         <v>80</v>
@@ -3066,10 +3049,10 @@
         <v>6</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="J97" s="1">
         <v>350</v>
@@ -3084,7 +3067,7 @@
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F98" s="1">
         <v>20</v>
@@ -3093,7 +3076,7 @@
         <v>6</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
@@ -3105,7 +3088,7 @@
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F99" s="1">
         <v>30</v>
@@ -3114,7 +3097,7 @@
         <v>6</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
@@ -3126,7 +3109,7 @@
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="F100" s="1">
         <v>10</v>
@@ -3135,7 +3118,7 @@
         <v>6</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
@@ -3147,12 +3130,12 @@
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
@@ -3164,7 +3147,7 @@
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="F102" s="1">
         <v>5</v>
@@ -3173,7 +3156,7 @@
         <v>6</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
@@ -3185,7 +3168,7 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
@@ -3199,16 +3182,16 @@
         <v>18</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C104" s="1">
         <v>20</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F104" s="1">
         <v>20</v>
@@ -3217,10 +3200,10 @@
         <v>6</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="J104" s="1">
         <v>350</v>
@@ -3235,7 +3218,7 @@
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F105" s="1">
         <v>65</v>
@@ -3244,7 +3227,7 @@
         <v>6</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
@@ -3256,7 +3239,7 @@
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F106" s="1">
         <v>75</v>
@@ -3265,7 +3248,7 @@
         <v>6</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
@@ -3277,7 +3260,7 @@
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F107" s="1">
         <v>220</v>
@@ -3286,7 +3269,7 @@
         <v>6</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
@@ -3298,7 +3281,7 @@
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F108" s="1">
         <v>10</v>
@@ -3307,7 +3290,7 @@
         <v>6</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
@@ -3319,7 +3302,7 @@
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>

</xml_diff>

<commit_message>
backend - 1# added snack to meals
</commit_message>
<xml_diff>
--- a/BackEnd/ExcelReader/src/main/resources/data/jadlospis2.xlsx
+++ b/BackEnd/ExcelReader/src/main/resources/data/jadlospis2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMOWANIE\etmeall2\EatMeAll\BackEnd\ExcelReader\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ADCC25-0059-4C3E-AA02-73A504309C0A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6828003F-0D64-4B4B-96FB-6834748AE67E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{DC9E3696-05CD-4AC0-85C8-C796492A84E0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="222">
   <si>
     <t>Koktajl mleczny z otrębami</t>
   </si>
@@ -372,39 +372,9 @@
     <t>X</t>
   </si>
   <si>
-    <t>szybki lunch 1</t>
-  </si>
-  <si>
-    <t>szybki lunch 2</t>
-  </si>
-  <si>
-    <t>szybki lunch 3</t>
-  </si>
-  <si>
     <t>banan</t>
   </si>
   <si>
-    <t>Malyszowe danie</t>
-  </si>
-  <si>
-    <t>Adam Malysz</t>
-  </si>
-  <si>
-    <t>Malysz wersja na kwasno</t>
-  </si>
-  <si>
-    <t>wiadro</t>
-  </si>
-  <si>
-    <t>wiaderko</t>
-  </si>
-  <si>
-    <t>Przeklaska Kwasniewskiego</t>
-  </si>
-  <si>
-    <t>Kwaśniewski</t>
-  </si>
-  <si>
     <t>ugotować ryż; wymieszać z mięsem mielonym z indyka, białkiem jaja i natką pietruszki; przyprawić solą i pieprzem; farszem wypełnić paprykę czerwoną; podlać 1 łyżką wody/bulionu; zapiekać w piekarniku nagrzanym do 200 stopni ok. 30-40 min; 10 min przed końcem posypać starym żółtym serem</t>
   </si>
   <si>
@@ -444,15 +414,6 @@
     <t>bułka grahamka</t>
   </si>
   <si>
-    <t>nutella</t>
-  </si>
-  <si>
-    <t>sledzik</t>
-  </si>
-  <si>
-    <t>kapusta kwaszona</t>
-  </si>
-  <si>
     <t>filet z piersi kurczaka</t>
   </si>
   <si>
@@ -493,13 +454,250 @@
   </si>
   <si>
     <t>ryż</t>
+  </si>
+  <si>
+    <t>Sałatka z pomidora, ogórka kiszonego  i cebulki</t>
+  </si>
+  <si>
+    <t>pomidory</t>
+  </si>
+  <si>
+    <t>ogórki kiszone/konserwowe</t>
+  </si>
+  <si>
+    <t>cebula</t>
+  </si>
+  <si>
+    <t>kilka piórek</t>
+  </si>
+  <si>
+    <t>grzybki marynowane</t>
+  </si>
+  <si>
+    <t>kilka szt.</t>
+  </si>
+  <si>
+    <t>oliwę z oliwek</t>
+  </si>
+  <si>
+    <t>pieczywo Wasa</t>
+  </si>
+  <si>
+    <t>3 kromki</t>
+  </si>
+  <si>
+    <t>pomidory ogórki kiszone/konserwowe, cebula, grzybki marynowane pokroić w kostkę; doprawić odrobiną soli, pieprzu; dodać oliwę z oliwek i ewentualnie pietruszkę; zjeść z pieczywem chrupkim Wasa</t>
+  </si>
+  <si>
+    <t>Jogurt pitny z waflami ryżowymi</t>
+  </si>
+  <si>
+    <t>Maślanka plus Batonik zbożowy</t>
+  </si>
+  <si>
+    <t>maślanka</t>
+  </si>
+  <si>
+    <t>batonik zbożowy</t>
+  </si>
+  <si>
+    <t>1 sz.</t>
+  </si>
+  <si>
+    <t>Jogurt pitny o dowolnym smaku; wafle ryżowe</t>
+  </si>
+  <si>
+    <t>Maślanka 0,5% tł;  batonik do wyboru: CiniMinis, Chocapic, Cheerios, Nesquick</t>
+  </si>
+  <si>
+    <t>KANAPKI Z SZYNKĄ, SAŁATĄ, POMIDOREM I AWOKADO</t>
+  </si>
+  <si>
+    <t>0,5 szt.</t>
+  </si>
+  <si>
+    <t>2 łyżeczki</t>
+  </si>
+  <si>
+    <t>4 x Plasterek</t>
+  </si>
+  <si>
+    <t>4 kromki</t>
+  </si>
+  <si>
+    <t>awokado</t>
+  </si>
+  <si>
+    <t>szynka z piersi kurczaka</t>
+  </si>
+  <si>
+    <t>4 liście</t>
+  </si>
+  <si>
+    <t>jabłko</t>
+  </si>
+  <si>
+    <t>chleb posmaruj masłem; na wierzch wyłóż sałatę, szynkę, plastry pomidora i cienkie plastry awokado; przypraw pieprzem; umyj jabłko i zjedz jako przekąskę</t>
+  </si>
+  <si>
+    <t>Łukasz Wiertel</t>
+  </si>
+  <si>
+    <t>KANAPKI Z MASŁEM ORZECHOWYM I BANANEM</t>
+  </si>
+  <si>
+    <t>masło orzechowe</t>
+  </si>
+  <si>
+    <t>Pieczywo posmaruj masłem orzechowym; Na wierzch wyłóż pokrojonego banana</t>
+  </si>
+  <si>
+    <t>przekąska</t>
+  </si>
+  <si>
+    <t>ORZECHY WŁOSKIE I DAKTYLE, SUSZONE</t>
+  </si>
+  <si>
+    <t>orzechy włoskie</t>
+  </si>
+  <si>
+    <t>daktyle, suszone</t>
+  </si>
+  <si>
+    <t>7 szt.</t>
+  </si>
+  <si>
+    <t>LECZO Z KURCZAKIEM I RYŻEM</t>
+  </si>
+  <si>
+    <t>1 łyżka</t>
+  </si>
+  <si>
+    <t>ryż brązowy</t>
+  </si>
+  <si>
+    <t>7 łyżek</t>
+  </si>
+  <si>
+    <t>koncentrat pomidorowy</t>
+  </si>
+  <si>
+    <t>2 porcji</t>
+  </si>
+  <si>
+    <t>cebulę posiekaj i wrzuć na rozgrzany olej; dodaj pokrojonego w kostkę kurczaka; cały czas mieszając podgrzewaj przez 5 minut. Następnie dodaj pokrojoną paprykę; po chwili dolej niewielką ilość wody i dodaj koncentrat; pomidory sparz, obierz, pokrój i dodaj do leczo; całość przypraw papryką słodką, chili, pieprzem i odrobiną soli (możesz dodać też np.oregano i rozmaryn); duś pod przykryciem przez kilka minut, aż papryka zmięknie; podawaj z ugotowanym ryżem</t>
+  </si>
+  <si>
+    <t>sok pomarańczowy</t>
+  </si>
+  <si>
+    <t>SAŁATKA CESAR ( Z KURCZAKIEM)</t>
+  </si>
+  <si>
+    <t>2 łyżeczka</t>
+  </si>
+  <si>
+    <t>1,2 porcji</t>
+  </si>
+  <si>
+    <t>6 liści</t>
+  </si>
+  <si>
+    <t>olowa z oliwek</t>
+  </si>
+  <si>
+    <t>sok z cytryny</t>
+  </si>
+  <si>
+    <t>oregano</t>
+  </si>
+  <si>
+    <t>filet zamarynuj w oregano i oliwie; dopraw solą i pieprzem; usmaż na patelni bez tłuszczowej lub wrzuć do wrzątku i ugotuj; pomidora pokrój, a sałatę podziel na mniejsze kawałki; wymieszaj wszystkie składniki i skrop oliwą; podawaj z pieczywem z masłem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pomarańczko </t>
+  </si>
+  <si>
+    <t>pomarańcze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pomidorki koktajlowe </t>
+  </si>
+  <si>
+    <t>pomidorki koktajlowe</t>
+  </si>
+  <si>
+    <t>6 szt.</t>
+  </si>
+  <si>
+    <t>Deser mleczny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gruszka </t>
+  </si>
+  <si>
+    <t>gruszka</t>
+  </si>
+  <si>
+    <t>Mandarynki</t>
+  </si>
+  <si>
+    <t>mandarynki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maślanka </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pieczywo chrupkie Wasa </t>
+  </si>
+  <si>
+    <t>4 szt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batonik musli </t>
+  </si>
+  <si>
+    <t>Twarożek ze szczypiorkiem</t>
+  </si>
+  <si>
+    <t>chudy twaróg</t>
+  </si>
+  <si>
+    <t>natka</t>
+  </si>
+  <si>
+    <t>3 szt/</t>
+  </si>
+  <si>
+    <t>Twarożek posiekać ze szczypiorkiem; dodać odrobina mleka 2% ; dodać kopiasta łyżka szczypiorku, sól; pieczywo chrupkie Wasa; przygryzac pomidorki koktajlowe</t>
+  </si>
+  <si>
+    <t>Ryż na mleku z owocami:</t>
+  </si>
+  <si>
+    <t>kiwi</t>
+  </si>
+  <si>
+    <t>nektarynka</t>
+  </si>
+  <si>
+    <t>1,5 szt.</t>
+  </si>
+  <si>
+    <t>ryż na mleku z owocami: biały ryż; ugotuj na mleku 2%, połącz z pokrojonymi w kostkę kiwi i nektarynką</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sałatka z pomidora i ogórka kiszonego </t>
+  </si>
+  <si>
+    <t>pomidory ogórki kiszone/konserwowe; grzybki marynowane pokroić w kostkę; doprawić odrobiną soli, pieprzu i oliwy z oliwek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,6 +712,23 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -551,11 +766,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,17 +1089,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1838D449-8DD4-4711-984B-E0AC88629B5C}">
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:K180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D177" sqref="D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="43.77734375" customWidth="1"/>
+    <col min="4" max="4" width="45.44140625" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" customWidth="1"/>
     <col min="9" max="9" width="78.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -889,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1">
         <v>10</v>
@@ -898,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1">
         <v>400</v>
@@ -919,7 +1138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -946,7 +1165,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F3" s="1">
         <v>100</v>
@@ -967,7 +1186,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F4" s="1">
         <v>200</v>
@@ -997,12 +1216,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1">
         <v>10</v>
@@ -1032,7 +1251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1053,7 +1272,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1074,7 +1293,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1110,12 +1329,12 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C11" s="1">
         <v>10</v>
@@ -1145,7 +1364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1166,7 +1385,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1228,7 +1447,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C16" s="1">
         <v>20</v>
@@ -1237,7 +1456,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="F16" s="1">
         <v>100</v>
@@ -1249,7 +1468,7 @@
         <v>21</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="J16" s="1">
         <v>300</v>
@@ -1355,12 +1574,12 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C22" s="1">
         <v>20</v>
@@ -1381,7 +1600,7 @@
         <v>29</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="J22" s="1">
         <v>300</v>
@@ -1396,7 +1615,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F23" s="1">
         <v>30</v>
@@ -1432,7 +1651,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1474,7 +1693,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1515,7 +1734,7 @@
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C29" s="1">
         <v>30</v>
@@ -1536,7 +1755,7 @@
         <v>39</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J29" s="1">
         <v>300</v>
@@ -1545,7 +1764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1566,7 +1785,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1623,7 +1842,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>7</v>
       </c>
@@ -1637,7 +1856,7 @@
         <v>45</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F34" s="1">
         <v>50</v>
@@ -1658,7 +1877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1721,7 +1940,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1742,7 +1961,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1792,7 +2011,7 @@
         <v>54</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F41" s="1">
         <v>160</v>
@@ -1813,7 +2032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1849,7 +2068,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>9</v>
       </c>
@@ -1863,7 +2082,7 @@
         <v>57</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="F44" s="1">
         <v>80</v>
@@ -1884,7 +2103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1947,7 +2166,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1983,7 +2202,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>10</v>
       </c>
@@ -1991,43 +2210,43 @@
         <v>63</v>
       </c>
       <c r="C50" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
       <c r="F50" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="J50" s="1">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="F51" s="1">
-        <v>500</v>
+        <v>120</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>6</v>
@@ -2045,49 +2264,41 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="F52" s="1">
+        <v>30</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="1">
-        <v>11</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" s="1">
-        <v>30</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>116</v>
-      </c>
+    <row r="53" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="F53" s="1">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="J53" s="1">
-        <v>300</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>120</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
     </row>
     <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
@@ -2095,16 +2306,16 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="F54" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
@@ -2116,49 +2327,41 @@
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="F55" s="1">
+        <v>40</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="1">
-        <v>12</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C56" s="1">
+    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F56" s="1">
         <v>30</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F56" s="1">
-        <v>200</v>
-      </c>
       <c r="G56" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J56" s="1">
-        <v>300</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>125</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
     </row>
     <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
@@ -2175,24 +2378,24 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58" s="1">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>65</v>
+        <v>154</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>142</v>
+        <v>53</v>
       </c>
       <c r="F58" s="1">
-        <v>150</v>
+        <v>330</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>6</v>
@@ -2201,10 +2404,10 @@
         <v>39</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="J58" s="1">
-        <v>600</v>
+        <v>350</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>4</v>
@@ -2216,62 +2419,70 @@
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F59" s="1">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F60" s="1">
-        <v>5</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
+    <row r="61" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>12</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="1">
+        <v>15</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="E61" s="1" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="F61" s="1">
-        <v>200</v>
+        <v>330</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J61" s="1">
+        <v>350</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="62" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
@@ -2279,62 +2490,70 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="F62" s="1">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F63" s="1">
-        <v>75</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
+    <row r="64" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>13</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C64" s="1">
+        <v>45</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="E64" s="1" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="F64" s="1">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J64" s="1">
+        <v>600</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="65" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
@@ -2342,49 +2561,41 @@
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="F65" s="1">
+        <v>150</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="1">
-        <v>14</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="1">
-        <v>45</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>70</v>
-      </c>
+    <row r="66" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="F66" s="1">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J66" s="1">
-        <v>600</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
     </row>
     <row r="67" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
@@ -2392,37 +2603,37 @@
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="F67" s="1">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="F68" s="1">
-        <v>55</v>
+        <v>200</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
@@ -2434,16 +2645,16 @@
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="F69" s="1">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
@@ -2458,13 +2669,13 @@
         <v>75</v>
       </c>
       <c r="F70" s="1">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
@@ -2476,58 +2687,66 @@
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F71" s="1">
-        <v>5</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
+    <row r="72" spans="1:11" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>14</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C72" s="1">
+        <v>45</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="E72" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F72" s="1">
-        <v>8</v>
+        <v>150</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-    </row>
-    <row r="73" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J72" s="1">
+        <v>600</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="F73" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
@@ -2539,36 +2758,38 @@
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="F74" s="1">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F75" s="1">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H75" s="1"/>
+      <c r="H75" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
@@ -2579,16 +2800,16 @@
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F76" s="1">
+        <v>40</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H76" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
@@ -2600,16 +2821,16 @@
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F77" s="1">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
@@ -2621,70 +2842,62 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F78" s="1">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="F79" s="1">
+        <v>15</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="1">
-        <v>15</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C80" s="1">
-        <v>45</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>87</v>
-      </c>
+    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
       <c r="E80" s="1" t="s">
-        <v>151</v>
+        <v>80</v>
       </c>
       <c r="F80" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="J80" s="1">
-        <v>600</v>
-      </c>
-      <c r="K80" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
     </row>
     <row r="81" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
@@ -2692,28 +2905,26 @@
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F81" s="1">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H81" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F82" s="1">
         <v>30</v>
@@ -2722,28 +2933,28 @@
         <v>6</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F83" s="1">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
@@ -2755,49 +2966,51 @@
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1" t="s">
-        <v>153</v>
+        <v>85</v>
       </c>
       <c r="F84" s="1">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F85" s="1">
-        <v>40</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
+    <row r="86" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>15</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C86" s="1">
+        <v>45</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="E86" s="1" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F86" s="1">
         <v>100</v>
@@ -2806,210 +3019,214 @@
         <v>6</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
-    </row>
-    <row r="87" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J86" s="1">
+        <v>600</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F87" s="1">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="F88" s="1">
+        <v>30</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="1">
-        <v>16</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C89" s="1">
-        <v>10</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>97</v>
-      </c>
+    <row r="89" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
       <c r="E89" s="1" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="F89" s="1">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I89" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J89" s="1">
-        <v>350</v>
-      </c>
-      <c r="K89" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+    </row>
+    <row r="90" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1" t="s">
-        <v>23</v>
+        <v>140</v>
       </c>
       <c r="F90" s="1">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>100</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="I90" s="1"/>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F91" s="1">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F92" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F93" s="1">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F94" s="1">
-        <v>25</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H94" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
+    <row r="95" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="1">
+        <v>16</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C95" s="1">
+        <v>10</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="E95" s="1" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="F95" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
-      <c r="K95" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J95" s="1">
+        <v>350</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="96" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="1"/>
@@ -3017,87 +3234,81 @@
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="F96" s="1">
+        <v>5</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="1">
-        <v>17</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C97" s="1">
-        <v>10</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>104</v>
-      </c>
+    <row r="97" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
       <c r="E97" s="1" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="F97" s="1">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J97" s="1">
-        <v>350</v>
-      </c>
-      <c r="K97" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+    </row>
+    <row r="98" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="F98" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>107</v>
+        <v>17</v>
       </c>
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
     </row>
-    <row r="99" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="F99" s="1">
+        <v>50</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H99" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
@@ -3109,89 +3320,99 @@
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F100" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
     </row>
-    <row r="101" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="F101" s="1">
+        <v>100</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H101" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
     </row>
-    <row r="102" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F102" s="1">
-        <v>5</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H102" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
     </row>
-    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
+    <row r="103" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="1">
+        <v>17</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C103" s="1">
+        <v>10</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="E103" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-      <c r="I103" s="1"/>
-      <c r="J103" s="1"/>
-      <c r="K103" s="1"/>
-    </row>
-    <row r="104" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="1">
-        <v>18</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C104" s="1">
-        <v>20</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>110</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="F103" s="1">
+        <v>80</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J103" s="1">
+        <v>350</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
       <c r="E104" s="1" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="F104" s="1">
         <v>20</v>
@@ -3200,97 +3421,87 @@
         <v>6</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I104" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J104" s="1">
-        <v>350</v>
-      </c>
-      <c r="K104" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+    </row>
+    <row r="105" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="F105" s="1">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
     </row>
-    <row r="106" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="F106" s="1">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
     </row>
-    <row r="107" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F107" s="1">
-        <v>220</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
       <c r="H107" s="1" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
     </row>
-    <row r="108" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="F108" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
@@ -3311,6 +3522,1633 @@
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
     </row>
+    <row r="110" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="1">
+        <v>18</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C110" s="1">
+        <v>20</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F110" s="1">
+        <v>20</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J110" s="1">
+        <v>350</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F111" s="1">
+        <v>65</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+    </row>
+    <row r="112" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F112" s="1">
+        <v>75</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+    </row>
+    <row r="113" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F113" s="1">
+        <v>220</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+    </row>
+    <row r="114" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F114" s="1">
+        <v>10</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+    </row>
+    <row r="115" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+    </row>
+    <row r="116" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="1">
+        <v>19</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C116" s="1">
+        <v>5</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E116" t="s">
+        <v>197</v>
+      </c>
+      <c r="F116" s="1">
+        <v>240</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J116" s="1">
+        <v>100</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+    </row>
+    <row r="118" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="1">
+        <v>20</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C118" s="1">
+        <v>5</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F118" s="1">
+        <v>150</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J118" s="1">
+        <v>100</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F119" s="1">
+        <v>20</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I119" s="1"/>
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+    </row>
+    <row r="120" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+    </row>
+    <row r="121" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="1">
+        <v>21</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C121" s="1">
+        <v>5</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F121" s="1">
+        <v>150</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J121" s="1">
+        <v>100</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+    </row>
+    <row r="123" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="1">
+        <v>22</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C123" s="1">
+        <v>5</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F123" s="1">
+        <v>200</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J123" s="1">
+        <v>100</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
+      <c r="J124" s="1"/>
+      <c r="K124" s="1"/>
+    </row>
+    <row r="125" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="1">
+        <v>23</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C125" s="1">
+        <v>5</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F125" s="1">
+        <v>250</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J125" s="1">
+        <v>100</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+      <c r="J126" s="1"/>
+      <c r="K126" s="1"/>
+    </row>
+    <row r="127" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="1">
+        <v>24</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C127" s="1">
+        <v>5</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F127" s="1">
+        <v>250</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J127" s="1">
+        <v>100</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
+      <c r="J128" s="1"/>
+      <c r="K128" s="1"/>
+    </row>
+    <row r="129" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="1">
+        <v>25</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C129" s="1">
+        <v>5</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F129" s="1">
+        <v>40</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J129" s="1">
+        <v>100</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+      <c r="I130" s="1"/>
+      <c r="J130" s="1"/>
+      <c r="K130" s="1"/>
+    </row>
+    <row r="131" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="1">
+        <v>26</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C131" s="1">
+        <v>5</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F131" s="1">
+        <v>25</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J131" s="1">
+        <v>100</v>
+      </c>
+      <c r="K131" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+    </row>
+    <row r="133" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="1">
+        <v>27</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C133" s="1">
+        <v>15</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F133" s="1">
+        <v>150</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I133" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J133" s="1">
+        <v>125</v>
+      </c>
+      <c r="K133" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+      <c r="E134" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F134" s="1">
+        <v>5</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I134" s="1"/>
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+    </row>
+    <row r="135" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F135" s="1">
+        <v>50</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+    </row>
+    <row r="136" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F136" s="1">
+        <v>20</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I136" s="1"/>
+      <c r="J136" s="1"/>
+      <c r="K136" s="1"/>
+    </row>
+    <row r="137" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F137" s="1">
+        <v>50</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I137" s="1"/>
+      <c r="J137" s="1"/>
+      <c r="K137" s="1"/>
+    </row>
+    <row r="138" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
+    </row>
+    <row r="139" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A139" s="1">
+        <v>28</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C139" s="1">
+        <v>15</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F139" s="1">
+        <v>25</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I139" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J139" s="1">
+        <v>125</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F140" s="1">
+        <v>250</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I140" s="2"/>
+      <c r="J140" s="2"/>
+      <c r="K140" s="2"/>
+    </row>
+    <row r="141" spans="1:11" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+      <c r="C141" s="1"/>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F141" s="1">
+        <v>35</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I141" s="2"/>
+      <c r="J141" s="2"/>
+      <c r="K141" s="2"/>
+    </row>
+    <row r="142" spans="1:11" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F142" s="1">
+        <v>60</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I142" s="2"/>
+      <c r="J142" s="2"/>
+      <c r="K142" s="2"/>
+    </row>
+    <row r="143" spans="1:11" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="1"/>
+      <c r="E143" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F143" s="1"/>
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+      <c r="I143" s="2"/>
+      <c r="J143" s="2"/>
+      <c r="K143" s="2"/>
+    </row>
+    <row r="144" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A144" s="1">
+        <v>29</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C144" s="1">
+        <v>15</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F144" s="1">
+        <v>300</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I144" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J144" s="1">
+        <v>125</v>
+      </c>
+      <c r="K144" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+      <c r="C145" s="1"/>
+      <c r="D145" s="1"/>
+      <c r="E145" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F145" s="1">
+        <v>120</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I145" s="1"/>
+      <c r="J145" s="1"/>
+      <c r="K145" s="1"/>
+    </row>
+    <row r="146" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+      <c r="E146" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F146" s="1">
+        <v>50</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H146" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I146" s="1"/>
+      <c r="J146" s="1"/>
+      <c r="K146" s="1"/>
+    </row>
+    <row r="147" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+      <c r="C147" s="1"/>
+      <c r="D147" s="1"/>
+      <c r="E147" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F147" s="1"/>
+      <c r="G147" s="1"/>
+      <c r="H147" s="1"/>
+      <c r="I147" s="1"/>
+      <c r="J147" s="1"/>
+      <c r="K147" s="1"/>
+    </row>
+    <row r="148" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="1">
+        <v>30</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C148" s="1">
+        <v>6</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F148" s="1">
+        <v>70</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H148" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I148" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J148" s="1">
+        <v>500</v>
+      </c>
+      <c r="K148" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="1"/>
+      <c r="E149" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F149" s="1">
+        <v>10</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I149" s="1"/>
+      <c r="J149" s="1"/>
+      <c r="K149" s="1"/>
+    </row>
+    <row r="150" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F150" s="1">
+        <v>60</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I150" s="1"/>
+      <c r="J150" s="1"/>
+      <c r="K150" s="1"/>
+    </row>
+    <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F151" s="1">
+        <v>120</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I151" s="1"/>
+      <c r="J151" s="1"/>
+      <c r="K151" s="1"/>
+    </row>
+    <row r="152" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F152" s="1">
+        <v>120</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H152" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I152" s="1"/>
+      <c r="J152" s="1"/>
+      <c r="K152" s="1"/>
+    </row>
+    <row r="153" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="1"/>
+      <c r="B153" s="1"/>
+      <c r="C153" s="1"/>
+      <c r="D153" s="1"/>
+      <c r="E153" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F153" s="1">
+        <v>20</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I153" s="1"/>
+      <c r="J153" s="1"/>
+      <c r="K153" s="1"/>
+    </row>
+    <row r="154" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
+      <c r="C154" s="1"/>
+      <c r="D154" s="1"/>
+      <c r="E154" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F154" s="1">
+        <v>120</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I154" s="1"/>
+      <c r="J154" s="1"/>
+      <c r="K154" s="1"/>
+    </row>
+    <row r="155" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
+      <c r="C155" s="1"/>
+      <c r="D155" s="1"/>
+      <c r="E155" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F155" s="1"/>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
+      <c r="I155" s="1"/>
+      <c r="J155" s="1"/>
+      <c r="K155" s="1"/>
+    </row>
+    <row r="156" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="1">
+        <v>31</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C156" s="1">
+        <v>6</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F156" s="1">
+        <v>90</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H156" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I156" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J156" s="1">
+        <v>837</v>
+      </c>
+      <c r="K156" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1"/>
+      <c r="E157" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F157" s="1">
+        <v>30</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H157" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I157" s="1"/>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1"/>
+    </row>
+    <row r="158" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
+      <c r="E158" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F158" s="1">
+        <v>120</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H158" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I158" s="1"/>
+      <c r="J158" s="1"/>
+      <c r="K158" s="1"/>
+    </row>
+    <row r="159" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="1"/>
+      <c r="D159" s="1"/>
+      <c r="E159" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F159" s="1"/>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1"/>
+      <c r="I159" s="1"/>
+      <c r="J159" s="1"/>
+      <c r="K159" s="1"/>
+    </row>
+    <row r="160" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A160" s="1">
+        <v>32</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C160" s="1">
+        <v>5</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F160" s="1">
+        <v>30</v>
+      </c>
+      <c r="G160" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H160" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I160" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J160" s="1">
+        <v>590</v>
+      </c>
+      <c r="K160" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1"/>
+      <c r="E161" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F161" s="1">
+        <v>35</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H161" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I161" s="1"/>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1"/>
+    </row>
+    <row r="162" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F162" s="1"/>
+      <c r="G162" s="1"/>
+      <c r="H162" s="1"/>
+      <c r="I162" s="1"/>
+      <c r="J162" s="1"/>
+      <c r="K162" s="1"/>
+    </row>
+    <row r="163" spans="1:11" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A163" s="1">
+        <v>33</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C163" s="1">
+        <v>40</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F163" s="1">
+        <v>10</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I163" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J163" s="1">
+        <v>300</v>
+      </c>
+      <c r="K163" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F164" s="1">
+        <v>100</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I164" s="1"/>
+      <c r="J164" s="1"/>
+      <c r="K164" s="1"/>
+    </row>
+    <row r="165" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F165" s="1">
+        <v>140</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I165" s="1"/>
+      <c r="J165" s="1"/>
+      <c r="K165" s="1"/>
+    </row>
+    <row r="166" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F166" s="1">
+        <v>140</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I166" s="1"/>
+      <c r="J166" s="1"/>
+      <c r="K166" s="1"/>
+    </row>
+    <row r="167" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F167" s="1">
+        <v>200</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I167" s="1"/>
+      <c r="J167" s="1"/>
+      <c r="K167" s="1"/>
+    </row>
+    <row r="168" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F168" s="1">
+        <v>120</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I168" s="1"/>
+      <c r="J168" s="1"/>
+      <c r="K168" s="1"/>
+    </row>
+    <row r="169" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
+      <c r="E169" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F169" s="1">
+        <v>50</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I169" s="1"/>
+      <c r="J169" s="1"/>
+      <c r="K169" s="1"/>
+    </row>
+    <row r="170" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F170" s="1">
+        <v>250</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I170" s="1"/>
+      <c r="J170" s="1"/>
+      <c r="K170" s="1"/>
+    </row>
+    <row r="171" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F171" s="1"/>
+      <c r="G171" s="1"/>
+      <c r="H171" s="1"/>
+      <c r="I171" s="1"/>
+      <c r="J171" s="1"/>
+      <c r="K171" s="1"/>
+    </row>
+    <row r="172" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A172" s="1">
+        <v>34</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C172" s="1">
+        <v>25</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F172" s="1">
+        <v>10</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I172" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J172" s="1">
+        <v>590</v>
+      </c>
+      <c r="K172" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1"/>
+      <c r="E173" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F173" s="1">
+        <v>120</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I173" s="1"/>
+      <c r="J173" s="1"/>
+      <c r="K173" s="1"/>
+    </row>
+    <row r="174" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F174" s="1">
+        <v>120</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H174" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I174" s="1"/>
+      <c r="J174" s="1"/>
+      <c r="K174" s="1"/>
+    </row>
+    <row r="175" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F175" s="1">
+        <v>30</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H175" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I175" s="1"/>
+      <c r="J175" s="1"/>
+      <c r="K175" s="1"/>
+    </row>
+    <row r="176" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F176" s="1">
+        <v>120</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I176" s="1"/>
+      <c r="J176" s="1"/>
+      <c r="K176" s="1"/>
+    </row>
+    <row r="177" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1"/>
+      <c r="E177" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F177" s="1">
+        <v>10</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I177" s="1"/>
+      <c r="J177" s="1"/>
+      <c r="K177" s="1"/>
+    </row>
+    <row r="178" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1"/>
+      <c r="E178" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F178" s="1">
+        <v>6</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I178" s="1"/>
+      <c r="J178" s="1"/>
+      <c r="K178" s="1"/>
+    </row>
+    <row r="179" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F179" s="1">
+        <v>2</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I179" s="1"/>
+      <c r="J179" s="1"/>
+      <c r="K179" s="1"/>
+    </row>
+    <row r="180" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F180" s="1"/>
+      <c r="G180" s="1"/>
+      <c r="H180" s="1"/>
+      <c r="I180" s="1"/>
+      <c r="J180" s="1"/>
+      <c r="K180" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
backend - 1# add Sknak do meals
</commit_message>
<xml_diff>
--- a/BackEnd/ExcelReader/src/main/resources/data/jadlospis2.xlsx
+++ b/BackEnd/ExcelReader/src/main/resources/data/jadlospis2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMOWANIE\etmeall2\EatMeAll\BackEnd\ExcelReader\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6828003F-0D64-4B4B-96FB-6834748AE67E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778E0234-22BD-4018-A2D8-D5A651E0DB8C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{DC9E3696-05CD-4AC0-85C8-C796492A84E0}"/>
   </bookViews>
@@ -273,9 +273,6 @@
     <t>mięso z piersi z kurczaka</t>
   </si>
   <si>
-    <t xml:space="preserve">cebulą </t>
-  </si>
-  <si>
     <t>1/4 szt</t>
   </si>
   <si>
@@ -691,6 +688,9 @@
   </si>
   <si>
     <t>pomidory ogórki kiszone/konserwowe; grzybki marynowane pokroić w kostkę; doprawić odrobiną soli, pieprzu i oliwy z oliwek</t>
+  </si>
+  <si>
+    <t>płatki owsiane</t>
   </si>
 </sst>
 </file>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1838D449-8DD4-4711-984B-E0AC88629B5C}">
   <dimension ref="A1:K180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D177" sqref="D177"/>
+    <sheetView tabSelected="1" topLeftCell="E73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1108,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1">
         <v>10</v>
@@ -1117,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F1" s="1">
         <v>400</v>
@@ -1165,7 +1165,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F3" s="1">
         <v>100</v>
@@ -1186,7 +1186,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F4" s="1">
         <v>200</v>
@@ -1207,7 +1207,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1221,7 +1221,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="1">
         <v>10</v>
@@ -1278,7 +1278,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="F8" s="1">
         <v>40</v>
@@ -1320,7 +1320,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1334,7 +1334,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="1">
         <v>10</v>
@@ -1433,7 +1433,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1447,7 +1447,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" s="1">
         <v>20</v>
@@ -1456,7 +1456,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F16" s="1">
         <v>100</v>
@@ -1468,7 +1468,7 @@
         <v>21</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J16" s="1">
         <v>300</v>
@@ -1483,7 +1483,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F17" s="1">
         <v>120</v>
@@ -1565,7 +1565,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1579,7 +1579,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C22" s="1">
         <v>20</v>
@@ -1600,7 +1600,7 @@
         <v>29</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J22" s="1">
         <v>300</v>
@@ -1615,7 +1615,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F23" s="1">
         <v>30</v>
@@ -1720,7 +1720,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1734,7 +1734,7 @@
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="1">
         <v>30</v>
@@ -1743,7 +1743,7 @@
         <v>38</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F29" s="1">
         <v>75</v>
@@ -1755,7 +1755,7 @@
         <v>39</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J29" s="1">
         <v>300</v>
@@ -1770,7 +1770,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F30" s="1">
         <v>80</v>
@@ -1833,7 +1833,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1856,7 +1856,7 @@
         <v>45</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F34" s="1">
         <v>50</v>
@@ -1988,7 +1988,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2011,7 +2011,7 @@
         <v>54</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F41" s="1">
         <v>160</v>
@@ -2059,7 +2059,7 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -2082,7 +2082,7 @@
         <v>57</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F44" s="1">
         <v>80</v>
@@ -2193,7 +2193,7 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2213,10 +2213,10 @@
         <v>15</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="F50" s="1">
         <v>300</v>
@@ -2228,7 +2228,7 @@
         <v>19</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J50" s="1">
         <v>350</v>
@@ -2243,7 +2243,7 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F51" s="1">
         <v>120</v>
@@ -2264,7 +2264,7 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F52" s="1">
         <v>30</v>
@@ -2273,7 +2273,7 @@
         <v>6</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
@@ -2285,7 +2285,7 @@
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F53" s="1">
         <v>50</v>
@@ -2294,7 +2294,7 @@
         <v>6</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
@@ -2306,7 +2306,7 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F54" s="1">
         <v>5</v>
@@ -2327,7 +2327,7 @@
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F55" s="1">
         <v>40</v>
@@ -2348,7 +2348,7 @@
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F56" s="1">
         <v>30</v>
@@ -2357,7 +2357,7 @@
         <v>6</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
@@ -2369,7 +2369,7 @@
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -2389,7 +2389,7 @@
         <v>15</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>53</v>
@@ -2404,7 +2404,7 @@
         <v>39</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J58" s="1">
         <v>350</v>
@@ -2440,7 +2440,7 @@
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -2460,10 +2460,10 @@
         <v>15</v>
       </c>
       <c r="D61" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="F61" s="1">
         <v>330</v>
@@ -2475,7 +2475,7 @@
         <v>39</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J61" s="1">
         <v>350</v>
@@ -2490,7 +2490,7 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F62" s="1">
         <v>25</v>
@@ -2499,7 +2499,7 @@
         <v>6</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -2511,7 +2511,7 @@
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -2534,7 +2534,7 @@
         <v>65</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F64" s="1">
         <v>150</v>
@@ -2546,7 +2546,7 @@
         <v>39</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J64" s="1">
         <v>600</v>
@@ -2582,7 +2582,7 @@
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F66" s="1">
         <v>5</v>
@@ -2603,7 +2603,7 @@
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F67" s="1">
         <v>200</v>
@@ -2624,7 +2624,7 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F68" s="1">
         <v>200</v>
@@ -2645,7 +2645,7 @@
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F69" s="1">
         <v>75</v>
@@ -2687,7 +2687,7 @@
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -2722,7 +2722,7 @@
         <v>72</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J72" s="1">
         <v>600</v>
@@ -2737,7 +2737,7 @@
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F73" s="1">
         <v>5</v>
@@ -2758,7 +2758,7 @@
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F74" s="1">
         <v>55</v>
@@ -2863,7 +2863,7 @@
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F79" s="1">
         <v>15</v>
@@ -2924,7 +2924,7 @@
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="F82" s="1">
         <v>30</v>
@@ -2933,7 +2933,7 @@
         <v>6</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
@@ -2945,7 +2945,7 @@
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F83" s="1">
         <v>75</v>
@@ -2966,7 +2966,7 @@
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F84" s="1">
         <v>20</v>
@@ -2975,7 +2975,7 @@
         <v>6</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
@@ -2987,7 +2987,7 @@
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -3007,10 +3007,10 @@
         <v>45</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F86" s="1">
         <v>100</v>
@@ -3022,7 +3022,7 @@
         <v>60</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J86" s="1">
         <v>600</v>
@@ -3037,7 +3037,7 @@
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F87" s="1">
         <v>10</v>
@@ -3058,7 +3058,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F88" s="1">
         <v>30</v>
@@ -3067,7 +3067,7 @@
         <v>6</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
@@ -3079,7 +3079,7 @@
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F89" s="1">
         <v>30</v>
@@ -3088,7 +3088,7 @@
         <v>6</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
@@ -3100,7 +3100,7 @@
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F90" s="1">
         <v>200</v>
@@ -3121,7 +3121,7 @@
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F91" s="1">
         <v>40</v>
@@ -3142,7 +3142,7 @@
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F92" s="1">
         <v>100</v>
@@ -3151,7 +3151,7 @@
         <v>6</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
@@ -3163,7 +3163,7 @@
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F93" s="1">
         <v>200</v>
@@ -3172,7 +3172,7 @@
         <v>1</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
@@ -3184,7 +3184,7 @@
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
@@ -3198,16 +3198,16 @@
         <v>16</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C95" s="1">
         <v>10</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F95" s="1">
         <v>80</v>
@@ -3219,7 +3219,7 @@
         <v>46</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J95" s="1">
         <v>350</v>
@@ -3243,10 +3243,10 @@
         <v>6</v>
       </c>
       <c r="H96" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I96" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
@@ -3257,7 +3257,7 @@
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F97" s="1">
         <v>50</v>
@@ -3278,7 +3278,7 @@
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F98" s="1">
         <v>30</v>
@@ -3299,7 +3299,7 @@
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F99" s="1">
         <v>50</v>
@@ -3329,7 +3329,7 @@
         <v>6</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
@@ -3341,7 +3341,7 @@
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F101" s="1">
         <v>100</v>
@@ -3362,7 +3362,7 @@
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
@@ -3376,16 +3376,16 @@
         <v>17</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C103" s="1">
         <v>10</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F103" s="1">
         <v>80</v>
@@ -3397,7 +3397,7 @@
         <v>42</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J103" s="1">
         <v>350</v>
@@ -3412,7 +3412,7 @@
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F104" s="1">
         <v>20</v>
@@ -3421,7 +3421,7 @@
         <v>6</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
@@ -3433,7 +3433,7 @@
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F105" s="1">
         <v>30</v>
@@ -3442,7 +3442,7 @@
         <v>6</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
@@ -3454,7 +3454,7 @@
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F106" s="1">
         <v>10</v>
@@ -3463,7 +3463,7 @@
         <v>6</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
@@ -3492,7 +3492,7 @@
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F108" s="1">
         <v>5</v>
@@ -3513,7 +3513,7 @@
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
@@ -3527,16 +3527,16 @@
         <v>18</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C110" s="1">
         <v>20</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F110" s="1">
         <v>20</v>
@@ -3545,10 +3545,10 @@
         <v>6</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J110" s="1">
         <v>350</v>
@@ -3563,7 +3563,7 @@
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F111" s="1">
         <v>65</v>
@@ -3572,7 +3572,7 @@
         <v>6</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
@@ -3584,7 +3584,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F112" s="1">
         <v>75</v>
@@ -3605,7 +3605,7 @@
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F113" s="1">
         <v>220</v>
@@ -3647,7 +3647,7 @@
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
@@ -3661,16 +3661,16 @@
         <v>19</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C116" s="1">
         <v>5</v>
       </c>
       <c r="D116" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E116" t="s">
         <v>196</v>
-      </c>
-      <c r="E116" t="s">
-        <v>197</v>
       </c>
       <c r="F116" s="1">
         <v>240</v>
@@ -3697,7 +3697,7 @@
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
@@ -3711,16 +3711,16 @@
         <v>20</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C118" s="1">
         <v>5</v>
       </c>
       <c r="D118" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="F118" s="1">
         <v>150</v>
@@ -3729,7 +3729,7 @@
         <v>6</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I118" s="1" t="s">
         <v>55</v>
@@ -3768,7 +3768,7 @@
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
@@ -3782,13 +3782,13 @@
         <v>21</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C121" s="1">
         <v>5</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>53</v>
@@ -3818,7 +3818,7 @@
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
@@ -3832,16 +3832,16 @@
         <v>22</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C123" s="1">
         <v>5</v>
       </c>
       <c r="D123" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E123" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="F123" s="1">
         <v>200</v>
@@ -3868,7 +3868,7 @@
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
@@ -3882,16 +3882,16 @@
         <v>23</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C125" s="1">
         <v>5</v>
       </c>
       <c r="D125" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E125" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="F125" s="1">
         <v>250</v>
@@ -3918,7 +3918,7 @@
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
@@ -3932,16 +3932,16 @@
         <v>24</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C127" s="1">
         <v>5</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F127" s="1">
         <v>250</v>
@@ -3968,7 +3968,7 @@
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
@@ -3982,16 +3982,16 @@
         <v>25</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C129" s="1">
         <v>5</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F129" s="1">
         <v>40</v>
@@ -4000,7 +4000,7 @@
         <v>6</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I129" s="1" t="s">
         <v>55</v>
@@ -4018,7 +4018,7 @@
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
@@ -4032,16 +4032,16 @@
         <v>26</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C131" s="1">
         <v>5</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F131" s="1">
         <v>25</v>
@@ -4068,7 +4068,7 @@
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
@@ -4082,16 +4082,16 @@
         <v>27</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C133" s="1">
         <v>15</v>
       </c>
       <c r="D133" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E133" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="F133" s="1">
         <v>150</v>
@@ -4103,7 +4103,7 @@
         <v>39</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J133" s="1">
         <v>125</v>
@@ -4118,7 +4118,7 @@
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F134" s="1">
         <v>5</v>
@@ -4127,7 +4127,7 @@
         <v>6</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I134" s="1"/>
       <c r="J134" s="1"/>
@@ -4139,7 +4139,7 @@
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F135" s="1">
         <v>50</v>
@@ -4148,7 +4148,7 @@
         <v>6</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I135" s="1"/>
       <c r="J135" s="1"/>
@@ -4160,7 +4160,7 @@
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F136" s="1">
         <v>20</v>
@@ -4181,7 +4181,7 @@
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F137" s="1">
         <v>50</v>
@@ -4190,7 +4190,7 @@
         <v>6</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I137" s="1"/>
       <c r="J137" s="1"/>
@@ -4202,7 +4202,7 @@
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
@@ -4216,16 +4216,16 @@
         <v>28</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C139" s="1">
         <v>15</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F139" s="1">
         <v>25</v>
@@ -4237,7 +4237,7 @@
         <v>17</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J139" s="1">
         <v>125</v>
@@ -4252,7 +4252,7 @@
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
       <c r="E140" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F140" s="1">
         <v>250</v>
@@ -4273,7 +4273,7 @@
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
       <c r="E141" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F141" s="1">
         <v>35</v>
@@ -4282,7 +4282,7 @@
         <v>6</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I141" s="2"/>
       <c r="J141" s="2"/>
@@ -4294,7 +4294,7 @@
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
       <c r="E142" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F142" s="1">
         <v>60</v>
@@ -4303,7 +4303,7 @@
         <v>6</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I142" s="2"/>
       <c r="J142" s="2"/>
@@ -4315,7 +4315,7 @@
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
@@ -4329,13 +4329,13 @@
         <v>29</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C144" s="1">
         <v>15</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>43</v>
@@ -4350,7 +4350,7 @@
         <v>52</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J144" s="1">
         <v>125</v>
@@ -4365,7 +4365,7 @@
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
       <c r="E145" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F145" s="1">
         <v>120</v>
@@ -4386,7 +4386,7 @@
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
       <c r="E146" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F146" s="1">
         <v>50</v>
@@ -4395,7 +4395,7 @@
         <v>6</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I146" s="1"/>
       <c r="J146" s="1"/>
@@ -4407,7 +4407,7 @@
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
       <c r="E147" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
@@ -4421,16 +4421,16 @@
         <v>30</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C148" s="1">
         <v>6</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F148" s="1">
         <v>70</v>
@@ -4439,16 +4439,16 @@
         <v>6</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J148" s="1">
         <v>500</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="149" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4466,7 +4466,7 @@
         <v>6</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I149" s="1"/>
       <c r="J149" s="1"/>
@@ -4478,7 +4478,7 @@
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
       <c r="E150" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F150" s="1">
         <v>60</v>
@@ -4487,7 +4487,7 @@
         <v>6</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I150" s="1"/>
       <c r="J150" s="1"/>
@@ -4499,7 +4499,7 @@
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
       <c r="E151" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F151" s="1">
         <v>120</v>
@@ -4508,7 +4508,7 @@
         <v>6</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I151" s="1"/>
       <c r="J151" s="1"/>
@@ -4550,7 +4550,7 @@
         <v>6</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I153" s="1"/>
       <c r="J153" s="1"/>
@@ -4562,7 +4562,7 @@
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
       <c r="E154" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F154" s="1">
         <v>120</v>
@@ -4583,7 +4583,7 @@
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
@@ -4603,10 +4603,10 @@
         <v>6</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F156" s="1">
         <v>90</v>
@@ -4615,16 +4615,16 @@
         <v>6</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J156" s="1">
         <v>837</v>
       </c>
       <c r="K156" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="157" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4633,7 +4633,7 @@
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
       <c r="E157" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F157" s="1">
         <v>30</v>
@@ -4642,7 +4642,7 @@
         <v>6</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I157" s="1"/>
       <c r="J157" s="1"/>
@@ -4654,7 +4654,7 @@
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
       <c r="E158" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F158" s="1">
         <v>120</v>
@@ -4675,7 +4675,7 @@
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
       <c r="E159" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
@@ -4689,16 +4689,16 @@
         <v>32</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C160" s="1">
         <v>5</v>
       </c>
       <c r="D160" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E160" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="F160" s="1">
         <v>30</v>
@@ -4716,7 +4716,7 @@
         <v>590</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="161" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4725,7 +4725,7 @@
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
       <c r="E161" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F161" s="1">
         <v>35</v>
@@ -4734,7 +4734,7 @@
         <v>6</v>
       </c>
       <c r="H161" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I161" s="1"/>
       <c r="J161" s="1"/>
@@ -4746,7 +4746,7 @@
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
       <c r="E162" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
@@ -4766,10 +4766,10 @@
         <v>40</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F163" s="1">
         <v>10</v>
@@ -4778,16 +4778,16 @@
         <v>6</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J163" s="1">
         <v>300</v>
       </c>
       <c r="K163" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="164" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4796,7 +4796,7 @@
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
       <c r="E164" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F164" s="1">
         <v>100</v>
@@ -4805,7 +4805,7 @@
         <v>6</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I164" s="1"/>
       <c r="J164" s="1"/>
@@ -4817,7 +4817,7 @@
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
       <c r="E165" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F165" s="1">
         <v>140</v>
@@ -4838,7 +4838,7 @@
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
       <c r="E166" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F166" s="1">
         <v>140</v>
@@ -4859,7 +4859,7 @@
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
       <c r="E167" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F167" s="1">
         <v>200</v>
@@ -4868,7 +4868,7 @@
         <v>6</v>
       </c>
       <c r="H167" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I167" s="1"/>
       <c r="J167" s="1"/>
@@ -4901,7 +4901,7 @@
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
       <c r="E169" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F169" s="1">
         <v>50</v>
@@ -4910,7 +4910,7 @@
         <v>6</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I169" s="1"/>
       <c r="J169" s="1"/>
@@ -4922,7 +4922,7 @@
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
       <c r="E170" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F170" s="1">
         <v>250</v>
@@ -4943,7 +4943,7 @@
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
       <c r="E171" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F171" s="1"/>
       <c r="G171" s="1"/>
@@ -4957,13 +4957,13 @@
         <v>34</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C172" s="1">
         <v>25</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>23</v>
@@ -4975,16 +4975,16 @@
         <v>6</v>
       </c>
       <c r="H172" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J172" s="1">
         <v>590</v>
       </c>
       <c r="K172" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="173" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4993,7 +4993,7 @@
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
       <c r="E173" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F173" s="1">
         <v>120</v>
@@ -5002,7 +5002,7 @@
         <v>6</v>
       </c>
       <c r="H173" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I173" s="1"/>
       <c r="J173" s="1"/>
@@ -5014,7 +5014,7 @@
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F174" s="1">
         <v>120</v>
@@ -5023,7 +5023,7 @@
         <v>6</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I174" s="1"/>
       <c r="J174" s="1"/>
@@ -5044,7 +5044,7 @@
         <v>6</v>
       </c>
       <c r="H175" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I175" s="1"/>
       <c r="J175" s="1"/>
@@ -5065,7 +5065,7 @@
         <v>6</v>
       </c>
       <c r="H176" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I176" s="1"/>
       <c r="J176" s="1"/>
@@ -5077,7 +5077,7 @@
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
       <c r="E177" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F177" s="1">
         <v>10</v>
@@ -5098,7 +5098,7 @@
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
       <c r="E178" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F178" s="1">
         <v>6</v>
@@ -5107,7 +5107,7 @@
         <v>6</v>
       </c>
       <c r="H178" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I178" s="1"/>
       <c r="J178" s="1"/>
@@ -5119,7 +5119,7 @@
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
       <c r="E179" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F179" s="1">
         <v>2</v>
@@ -5140,7 +5140,7 @@
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
       <c r="E180" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F180" s="1"/>
       <c r="G180" s="1"/>

</xml_diff>

<commit_message>
backend -- 1# added new meals to excel
</commit_message>
<xml_diff>
--- a/BackEnd/ExcelReader/src/main/resources/data/jadlospis2.xlsx
+++ b/BackEnd/ExcelReader/src/main/resources/data/jadlospis2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMOWANIE\etmeall2\EatMeAll\BackEnd\ExcelReader\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6828003F-0D64-4B4B-96FB-6834748AE67E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC76115-FEAC-4FB2-8387-16FD70ABBBD4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{DC9E3696-05CD-4AC0-85C8-C796492A84E0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="251">
   <si>
     <t>Koktajl mleczny z otrębami</t>
   </si>
@@ -691,6 +691,93 @@
   </si>
   <si>
     <t>pomidory ogórki kiszone/konserwowe; grzybki marynowane pokroić w kostkę; doprawić odrobiną soli, pieprzu i oliwy z oliwek</t>
+  </si>
+  <si>
+    <t>majonez</t>
+  </si>
+  <si>
+    <t>JAJKA NA TWARDO i KANAPKA Z HUMMUSEM</t>
+  </si>
+  <si>
+    <t>hummus klasyczny</t>
+  </si>
+  <si>
+    <t>szpinak</t>
+  </si>
+  <si>
+    <t>1 garść</t>
+  </si>
+  <si>
+    <t>zagotuj osoloną wodę; wrzuć jajka i nie przerywając wrzenia gotuj przez 8 min; ostudź i usuń skorupkę; na wierzch wyłóż majonez; chleb posmaruj hummusem; na wierzch wyłóż szpinak i szynkę</t>
+  </si>
+  <si>
+    <t>JOGURT Z MUSLI I BANANEM</t>
+  </si>
+  <si>
+    <t>musli z rodzynkami i orzechami</t>
+  </si>
+  <si>
+    <t>8 łyżek</t>
+  </si>
+  <si>
+    <t>9 łyżek</t>
+  </si>
+  <si>
+    <t>wymieszaj jogurt z musli; dodaj pokrojonego banana</t>
+  </si>
+  <si>
+    <t>MAKARON Z PESTO, SZPINAKIEM I KURCZAKIEM</t>
+  </si>
+  <si>
+    <t>pesto zielone z bazylii</t>
+  </si>
+  <si>
+    <t>makaron pełnoziarnisty</t>
+  </si>
+  <si>
+    <t>1, 8 szklanki</t>
+  </si>
+  <si>
+    <t>pierś z kurczaka</t>
+  </si>
+  <si>
+    <t>2 porcje</t>
+  </si>
+  <si>
+    <t>pomidory koktajlowe</t>
+  </si>
+  <si>
+    <t>dynia, pestki, łuskane</t>
+  </si>
+  <si>
+    <t>0.5 łyzki</t>
+  </si>
+  <si>
+    <t>ugotuj makaron; mięso pokrój w kostkę, przypraw ziołami oraz solą; natrzyj olejem, zwiń w folię do pieczenia; upiecz w piekarniku (około 20 minut); makaron wymieszaj z pesto, szpinakiem, mięsem, pestkami dyni oraz pomidorkami koktajlowymi</t>
+  </si>
+  <si>
+    <t>MORELE, SUSZONE</t>
+  </si>
+  <si>
+    <t>morele suszone</t>
+  </si>
+  <si>
+    <t>13 szt.</t>
+  </si>
+  <si>
+    <t>TWAROŻEK ZE SZCZYPIORKIEM</t>
+  </si>
+  <si>
+    <t>ser twaróg chudy</t>
+  </si>
+  <si>
+    <t>0,5 opakowania</t>
+  </si>
+  <si>
+    <t>1 sztuka</t>
+  </si>
+  <si>
+    <t>rozdrobnij widelcem twaróg i wymieszaj z twarogiem; dodaj posiekany szczypiorek; dopraw serek za pomocą ziół i pieprzu; podawaj z pieczywem z masłem</t>
   </si>
 </sst>
 </file>
@@ -1089,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1838D449-8DD4-4711-984B-E0AC88629B5C}">
-  <dimension ref="A1:K180"/>
+  <dimension ref="A1:K208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D177" sqref="D177"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K203" sqref="K203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5149,6 +5236,634 @@
       <c r="J180" s="1"/>
       <c r="K180" s="1"/>
     </row>
+    <row r="181" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A181" s="1">
+        <v>35</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C181" s="1">
+        <v>20</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F181" s="1">
+        <v>30</v>
+      </c>
+      <c r="G181" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H181" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I181" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J181" s="1">
+        <v>606</v>
+      </c>
+      <c r="K181" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
+      <c r="C182" s="1"/>
+      <c r="D182" s="1"/>
+      <c r="E182" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F182" s="1">
+        <v>112</v>
+      </c>
+      <c r="G182" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I182" s="1"/>
+      <c r="J182" s="1"/>
+      <c r="K182" s="1"/>
+    </row>
+    <row r="183" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
+      <c r="C183" s="1"/>
+      <c r="D183" s="1"/>
+      <c r="E183" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F183" s="1">
+        <v>60</v>
+      </c>
+      <c r="G183" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H183" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I183" s="1"/>
+      <c r="J183" s="1"/>
+      <c r="K183" s="1"/>
+    </row>
+    <row r="184" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1"/>
+      <c r="D184" s="1"/>
+      <c r="E184" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F184" s="1">
+        <v>20</v>
+      </c>
+      <c r="G184" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H184" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I184" s="1"/>
+      <c r="J184" s="1"/>
+      <c r="K184" s="1"/>
+    </row>
+    <row r="185" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A185" s="1"/>
+      <c r="B185" s="1"/>
+      <c r="C185" s="1"/>
+      <c r="D185" s="1"/>
+      <c r="E185" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F185" s="1">
+        <v>25</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H185" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="I185" s="1"/>
+      <c r="J185" s="1"/>
+      <c r="K185" s="1"/>
+    </row>
+    <row r="186" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A186" s="1"/>
+      <c r="B186" s="1"/>
+      <c r="C186" s="1"/>
+      <c r="D186" s="1"/>
+      <c r="E186" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F186" s="1">
+        <v>30</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H186" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I186" s="1"/>
+      <c r="J186" s="1"/>
+      <c r="K186" s="1"/>
+    </row>
+    <row r="187" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A187" s="1"/>
+      <c r="B187" s="1"/>
+      <c r="C187" s="1"/>
+      <c r="D187" s="1"/>
+      <c r="E187" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F187" s="1"/>
+      <c r="G187" s="1"/>
+      <c r="H187" s="1"/>
+      <c r="I187" s="1"/>
+      <c r="J187" s="1"/>
+      <c r="K187" s="1"/>
+    </row>
+    <row r="188" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A188" s="1">
+        <v>36</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C188" s="1">
+        <v>5</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F188" s="1">
+        <v>120</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H188" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I188" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J188" s="1">
+        <v>538</v>
+      </c>
+      <c r="K188" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A189" s="1"/>
+      <c r="B189" s="1"/>
+      <c r="C189" s="1"/>
+      <c r="D189" s="1"/>
+      <c r="E189" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F189" s="1">
+        <v>80</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H189" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I189" s="1"/>
+      <c r="J189" s="1"/>
+      <c r="K189" s="1"/>
+    </row>
+    <row r="190" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A190" s="1"/>
+      <c r="B190" s="1"/>
+      <c r="C190" s="1"/>
+      <c r="D190" s="1"/>
+      <c r="E190" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F190" s="1">
+        <v>180</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H190" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I190" s="1"/>
+      <c r="J190" s="1"/>
+      <c r="K190" s="1"/>
+    </row>
+    <row r="191" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A191" s="1"/>
+      <c r="B191" s="1"/>
+      <c r="C191" s="1"/>
+      <c r="D191" s="1"/>
+      <c r="E191" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F191" s="1"/>
+      <c r="G191" s="1"/>
+      <c r="H191" s="1"/>
+      <c r="I191" s="1"/>
+      <c r="J191" s="1"/>
+      <c r="K191" s="1"/>
+    </row>
+    <row r="192" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A192" s="1">
+        <v>37</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C192" s="1">
+        <v>30</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F192" s="1">
+        <v>25</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H192" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="I192" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="J192" s="1">
+        <v>900</v>
+      </c>
+      <c r="K192" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A193" s="1"/>
+      <c r="B193" s="1"/>
+      <c r="C193" s="1"/>
+      <c r="D193" s="1"/>
+      <c r="E193" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F193" s="1">
+        <v>40</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H193" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I193" s="1"/>
+      <c r="J193" s="1"/>
+      <c r="K193" s="1"/>
+    </row>
+    <row r="194" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A194" s="1"/>
+      <c r="B194" s="1"/>
+      <c r="C194" s="1"/>
+      <c r="D194" s="1"/>
+      <c r="E194" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F194" s="1">
+        <v>40</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H194" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I194" s="1"/>
+      <c r="J194" s="1"/>
+      <c r="K194" s="1"/>
+    </row>
+    <row r="195" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A195" s="1"/>
+      <c r="B195" s="1"/>
+      <c r="C195" s="1"/>
+      <c r="D195" s="1"/>
+      <c r="E195" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F195" s="1">
+        <v>200</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H195" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="I195" s="1"/>
+      <c r="J195" s="1"/>
+      <c r="K195" s="1"/>
+    </row>
+    <row r="196" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A196" s="1"/>
+      <c r="B196" s="1"/>
+      <c r="C196" s="1"/>
+      <c r="D196" s="1"/>
+      <c r="E196" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F196" s="1">
+        <v>60</v>
+      </c>
+      <c r="G196" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H196" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I196" s="1"/>
+      <c r="J196" s="1"/>
+      <c r="K196" s="1"/>
+    </row>
+    <row r="197" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A197" s="1"/>
+      <c r="B197" s="1"/>
+      <c r="C197" s="1"/>
+      <c r="D197" s="1"/>
+      <c r="E197" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F197" s="1">
+        <v>10</v>
+      </c>
+      <c r="G197" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H197" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I197" s="1"/>
+      <c r="J197" s="1"/>
+      <c r="K197" s="1"/>
+    </row>
+    <row r="198" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A198" s="1"/>
+      <c r="B198" s="1"/>
+      <c r="C198" s="1"/>
+      <c r="D198" s="1"/>
+      <c r="E198" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F198" s="1">
+        <v>5</v>
+      </c>
+      <c r="G198" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H198" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I198" s="1"/>
+      <c r="J198" s="1"/>
+      <c r="K198" s="1"/>
+    </row>
+    <row r="199" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A199" s="1"/>
+      <c r="B199" s="1"/>
+      <c r="C199" s="1"/>
+      <c r="D199" s="1"/>
+      <c r="E199" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F199" s="1"/>
+      <c r="G199" s="1"/>
+      <c r="H199" s="1"/>
+      <c r="I199" s="1"/>
+      <c r="J199" s="1"/>
+      <c r="K199" s="1"/>
+    </row>
+    <row r="200" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A200" s="1">
+        <v>38</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C200" s="1">
+        <v>1</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F200" s="1">
+        <v>100</v>
+      </c>
+      <c r="G200" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H200" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="I200" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J200" s="1">
+        <v>300</v>
+      </c>
+      <c r="K200" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A201" s="1"/>
+      <c r="B201" s="1"/>
+      <c r="C201" s="1"/>
+      <c r="D201" s="1"/>
+      <c r="E201" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F201" s="1"/>
+      <c r="G201" s="1"/>
+      <c r="H201" s="1"/>
+      <c r="I201" s="1"/>
+      <c r="J201" s="1"/>
+      <c r="K201" s="1"/>
+    </row>
+    <row r="202" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A202" s="1">
+        <v>39</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C202" s="1">
+        <v>7</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F202" s="1">
+        <v>10</v>
+      </c>
+      <c r="G202" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H202" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I202" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J202" s="1">
+        <v>590</v>
+      </c>
+      <c r="K202" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A203" s="1"/>
+      <c r="B203" s="1"/>
+      <c r="C203" s="1"/>
+      <c r="D203" s="1"/>
+      <c r="E203" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F203" s="1">
+        <v>120</v>
+      </c>
+      <c r="G203" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H203" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I203" s="1"/>
+      <c r="J203" s="1"/>
+      <c r="K203" s="1"/>
+    </row>
+    <row r="204" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
+      <c r="C204" s="1"/>
+      <c r="D204" s="1"/>
+      <c r="E204" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F204" s="1">
+        <v>100</v>
+      </c>
+      <c r="G204" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H204" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="I204" s="1"/>
+      <c r="J204" s="1"/>
+      <c r="K204" s="1"/>
+    </row>
+    <row r="205" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A205" s="1"/>
+      <c r="B205" s="1"/>
+      <c r="C205" s="1"/>
+      <c r="D205" s="1"/>
+      <c r="E205" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F205" s="1">
+        <v>80</v>
+      </c>
+      <c r="G205" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H205" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I205" s="1"/>
+      <c r="J205" s="1"/>
+      <c r="K205" s="1"/>
+    </row>
+    <row r="206" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A206" s="1"/>
+      <c r="B206" s="1"/>
+      <c r="C206" s="1"/>
+      <c r="D206" s="1"/>
+      <c r="E206" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F206" s="1">
+        <v>10</v>
+      </c>
+      <c r="G206" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H206" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I206" s="1"/>
+      <c r="J206" s="1"/>
+      <c r="K206" s="1"/>
+    </row>
+    <row r="207" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A207" s="1"/>
+      <c r="B207" s="1"/>
+      <c r="C207" s="1"/>
+      <c r="D207" s="1"/>
+      <c r="E207" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F207" s="1">
+        <v>200</v>
+      </c>
+      <c r="G207" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H207" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I207" s="1"/>
+      <c r="J207" s="1"/>
+      <c r="K207" s="1"/>
+    </row>
+    <row r="208" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A208" s="1"/>
+      <c r="B208" s="1"/>
+      <c r="C208" s="1"/>
+      <c r="D208" s="1"/>
+      <c r="E208" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F208" s="1"/>
+      <c r="G208" s="1"/>
+      <c r="H208" s="1"/>
+      <c r="I208" s="1"/>
+      <c r="J208" s="1"/>
+      <c r="K208" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1# excel fixed cell
</commit_message>
<xml_diff>
--- a/BackEnd/ExcelReader/src/main/resources/data/jadlospis2.xlsx
+++ b/BackEnd/ExcelReader/src/main/resources/data/jadlospis2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMOWANIE\etmeall2\EatMeAll\BackEnd\ExcelReader\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9349D5AD-1785-452B-BB3B-3AEC0AF7A821}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCDDD9E-F2AD-495A-9BCE-AE32B3A39BB5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{DC9E3696-05CD-4AC0-85C8-C796492A84E0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5958" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5954" uniqueCount="501">
   <si>
     <t>ml</t>
   </si>
@@ -1024,9 +1024,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>jogurt owocowy z suszonymi owocami</t>
@@ -1543,13 +1540,13 @@
     <t>wymieszaj jogurt z musli</t>
   </si>
   <si>
-    <t>sałatka z pomidorem, ogórkiem, sałatą i mozzarelląsałata</t>
-  </si>
-  <si>
     <t>pokrój pomidora, cebulę i ogórka; wymieszaj warzywa oraz dodaj porwane na mniejsze części liście sałaty; dodaj kawałki mozzarelli, oliwę oraz pieprz i sól. wymieszaj; podawaj z pieczywem z masłem</t>
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>sałatka z pomidorem, ogórkiem, sałatą i mozzarellą sałata</t>
   </si>
 </sst>
 </file>
@@ -1939,8 +1936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1838D449-8DD4-4711-984B-E0AC88629B5C}">
   <dimension ref="A1:K615"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A601" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D606" sqref="D606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2106,7 +2103,7 @@
         <v>332</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>332</v>
@@ -2138,7 +2135,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>42</v>
@@ -2153,7 +2150,7 @@
         <v>7</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J6" s="2">
         <v>300</v>
@@ -2185,7 +2182,7 @@
         <v>4</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>332</v>
@@ -2281,7 +2278,7 @@
         <v>332</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>332</v>
@@ -2313,7 +2310,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>42</v>
@@ -2328,7 +2325,7 @@
         <v>7</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J11" s="2">
         <v>300</v>
@@ -2456,7 +2453,7 @@
         <v>332</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>332</v>
@@ -2488,7 +2485,7 @@
         <v>20</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>111</v>
@@ -2503,7 +2500,7 @@
         <v>15</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J16" s="2">
         <v>300</v>
@@ -2640,7 +2637,7 @@
         <v>4</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>332</v>
@@ -2666,7 +2663,7 @@
         <v>332</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>332</v>
@@ -2698,7 +2695,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>20</v>
@@ -2713,7 +2710,7 @@
         <v>21</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J22" s="2">
         <v>300</v>
@@ -2911,7 +2908,7 @@
         <v>332</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>332</v>
@@ -2943,7 +2940,7 @@
         <v>30</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>68</v>
@@ -3086,7 +3083,7 @@
         <v>332</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>332</v>
@@ -3118,7 +3115,7 @@
         <v>15</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>99</v>
@@ -3133,7 +3130,7 @@
         <v>36</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J34" s="2">
         <v>350</v>
@@ -3331,7 +3328,7 @@
         <v>332</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>332</v>
@@ -3363,7 +3360,7 @@
         <v>15</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>92</v>
@@ -3378,7 +3375,7 @@
         <v>41</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J41" s="2">
         <v>350</v>
@@ -3436,7 +3433,7 @@
         <v>332</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>332</v>
@@ -3468,7 +3465,7 @@
         <v>15</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>100</v>
@@ -3483,7 +3480,7 @@
         <v>30</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J44" s="2">
         <v>350</v>
@@ -3646,7 +3643,7 @@
         <v>332</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>332</v>
@@ -3678,7 +3675,7 @@
         <v>15</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>34</v>
@@ -3693,7 +3690,7 @@
         <v>14</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J50" s="2">
         <v>350</v>
@@ -3891,7 +3888,7 @@
         <v>332</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F56" s="2">
         <v>30</v>
@@ -3926,7 +3923,7 @@
         <v>332</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>332</v>
@@ -3958,7 +3955,7 @@
         <v>15</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>42</v>
@@ -3973,7 +3970,7 @@
         <v>30</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J58" s="2">
         <v>350</v>
@@ -4031,7 +4028,7 @@
         <v>332</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>332</v>
@@ -4063,7 +4060,7 @@
         <v>15</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>122</v>
@@ -4078,7 +4075,7 @@
         <v>30</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J61" s="2">
         <v>350</v>
@@ -4136,7 +4133,7 @@
         <v>332</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>332</v>
@@ -4168,7 +4165,7 @@
         <v>45</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>101</v>
@@ -4183,7 +4180,7 @@
         <v>30</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J64" s="2">
         <v>600</v>
@@ -4416,7 +4413,7 @@
         <v>332</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>332</v>
@@ -4448,7 +4445,7 @@
         <v>45</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>55</v>
@@ -4463,7 +4460,7 @@
         <v>56</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J72" s="2">
         <v>600</v>
@@ -4775,7 +4772,7 @@
         <v>4</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>332</v>
+        <v>30</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>332</v>
@@ -4906,7 +4903,7 @@
         <v>332</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>332</v>
@@ -4938,7 +4935,7 @@
         <v>45</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>110</v>
@@ -4953,7 +4950,7 @@
         <v>46</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J86" s="2">
         <v>600</v>
@@ -5221,7 +5218,7 @@
         <v>332</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>332</v>
@@ -5253,7 +5250,7 @@
         <v>10</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>99</v>
@@ -5268,7 +5265,7 @@
         <v>36</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J95" s="2">
         <v>350</v>
@@ -5501,7 +5498,7 @@
         <v>332</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>332</v>
@@ -5533,7 +5530,7 @@
         <v>10</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>99</v>
@@ -5548,7 +5545,7 @@
         <v>33</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J103" s="2">
         <v>350</v>
@@ -5678,11 +5675,11 @@
       <c r="E107" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F107" s="2" t="s">
-        <v>332</v>
+      <c r="F107" s="2">
+        <v>10</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>332</v>
+        <v>4</v>
       </c>
       <c r="H107" s="2" t="s">
         <v>47</v>
@@ -5746,7 +5743,7 @@
         <v>332</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>332</v>
@@ -5778,7 +5775,7 @@
         <v>20</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>114</v>
@@ -5956,7 +5953,7 @@
         <v>332</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>332</v>
@@ -5988,7 +5985,7 @@
         <v>5</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>151</v>
@@ -6003,7 +6000,7 @@
         <v>30</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J116" s="2">
         <v>100</v>
@@ -6026,7 +6023,7 @@
         <v>332</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>332</v>
@@ -6058,7 +6055,7 @@
         <v>5</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>152</v>
@@ -6073,7 +6070,7 @@
         <v>153</v>
       </c>
       <c r="I118" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J118" s="2">
         <v>100</v>
@@ -6131,7 +6128,7 @@
         <v>332</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>332</v>
@@ -6163,7 +6160,7 @@
         <v>5</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>42</v>
@@ -6178,7 +6175,7 @@
         <v>30</v>
       </c>
       <c r="I121" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J121" s="2">
         <v>100</v>
@@ -6201,7 +6198,7 @@
         <v>332</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F122" s="2" t="s">
         <v>332</v>
@@ -6233,7 +6230,7 @@
         <v>5</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>154</v>
@@ -6248,7 +6245,7 @@
         <v>30</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J123" s="2">
         <v>100</v>
@@ -6271,7 +6268,7 @@
         <v>332</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F124" s="2" t="s">
         <v>332</v>
@@ -6318,7 +6315,7 @@
         <v>14</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J125" s="2">
         <v>100</v>
@@ -6341,7 +6338,7 @@
         <v>332</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F126" s="2" t="s">
         <v>332</v>
@@ -6373,7 +6370,7 @@
         <v>5</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>122</v>
@@ -6388,7 +6385,7 @@
         <v>30</v>
       </c>
       <c r="I127" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J127" s="2">
         <v>100</v>
@@ -6411,7 +6408,7 @@
         <v>332</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>332</v>
@@ -6443,10 +6440,10 @@
         <v>5</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F129" s="2">
         <v>40</v>
@@ -6458,7 +6455,7 @@
         <v>156</v>
       </c>
       <c r="I129" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J129" s="2">
         <v>100</v>
@@ -6481,7 +6478,7 @@
         <v>332</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F130" s="2" t="s">
         <v>332</v>
@@ -6513,7 +6510,7 @@
         <v>5</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>123</v>
@@ -6528,7 +6525,7 @@
         <v>30</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J131" s="2">
         <v>100</v>
@@ -6551,7 +6548,7 @@
         <v>332</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>332</v>
@@ -6583,7 +6580,7 @@
         <v>15</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>157</v>
@@ -6598,7 +6595,7 @@
         <v>30</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J133" s="2">
         <v>125</v>
@@ -6691,7 +6688,7 @@
         <v>332</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F136" s="2">
         <v>20</v>
@@ -6761,7 +6758,7 @@
         <v>332</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F138" s="2" t="s">
         <v>332</v>
@@ -6793,7 +6790,7 @@
         <v>15</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>114</v>
@@ -6936,7 +6933,7 @@
         <v>332</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F143" s="2" t="s">
         <v>332</v>
@@ -6968,7 +6965,7 @@
         <v>15</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>34</v>
@@ -7076,7 +7073,7 @@
         <v>332</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>332</v>
@@ -7108,7 +7105,7 @@
         <v>6</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>128</v>
@@ -7129,7 +7126,7 @@
         <v>500</v>
       </c>
       <c r="K148" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="149" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7190,7 +7187,7 @@
         <v>4</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I150" s="2" t="s">
         <v>332</v>
@@ -7356,7 +7353,7 @@
         <v>332</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F155" s="2" t="s">
         <v>332</v>
@@ -7388,7 +7385,7 @@
         <v>6</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>99</v>
@@ -7403,13 +7400,13 @@
         <v>121</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J156" s="2">
         <v>837</v>
       </c>
       <c r="K156" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="157" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7496,7 +7493,7 @@
         <v>332</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>332</v>
@@ -7528,7 +7525,7 @@
         <v>5</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>135</v>
@@ -7543,13 +7540,13 @@
         <v>12</v>
       </c>
       <c r="I160" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J160" s="2">
         <v>590</v>
       </c>
       <c r="K160" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="161" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7601,7 +7598,7 @@
         <v>332</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>332</v>
@@ -7633,7 +7630,7 @@
         <v>40</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>102</v>
@@ -7648,13 +7645,13 @@
         <v>138</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J163" s="2">
         <v>300</v>
       </c>
       <c r="K163" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="164" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7916,7 +7913,7 @@
         <v>332</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F171" s="2" t="s">
         <v>332</v>
@@ -7948,7 +7945,7 @@
         <v>25</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E172" s="2" t="s">
         <v>17</v>
@@ -7969,7 +7966,7 @@
         <v>590</v>
       </c>
       <c r="K172" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="173" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8231,7 +8228,7 @@
         <v>332</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F180" s="2" t="s">
         <v>332</v>
@@ -8263,7 +8260,7 @@
         <v>20</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E181" s="2" t="s">
         <v>165</v>
@@ -8284,7 +8281,7 @@
         <v>606</v>
       </c>
       <c r="K181" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="182" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8476,7 +8473,7 @@
         <v>332</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F187" s="2" t="s">
         <v>332</v>
@@ -8508,7 +8505,7 @@
         <v>5</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E188" s="2" t="s">
         <v>92</v>
@@ -8529,7 +8526,7 @@
         <v>538</v>
       </c>
       <c r="K188" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="189" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8616,7 +8613,7 @@
         <v>332</v>
       </c>
       <c r="E191" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F191" s="2" t="s">
         <v>332</v>
@@ -8648,7 +8645,7 @@
         <v>30</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E192" s="2" t="s">
         <v>167</v>
@@ -8669,7 +8666,7 @@
         <v>900</v>
       </c>
       <c r="K192" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="193" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8896,7 +8893,7 @@
         <v>332</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F199" s="2" t="s">
         <v>332</v>
@@ -8928,7 +8925,7 @@
         <v>1</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E200" s="2" t="s">
         <v>183</v>
@@ -8943,13 +8940,13 @@
         <v>184</v>
       </c>
       <c r="I200" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J200" s="2">
         <v>300</v>
       </c>
       <c r="K200" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="201" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8966,7 +8963,7 @@
         <v>332</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F201" s="2" t="s">
         <v>332</v>
@@ -8998,7 +8995,7 @@
         <v>7</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E202" s="2" t="s">
         <v>17</v>
@@ -9019,7 +9016,7 @@
         <v>590</v>
       </c>
       <c r="K202" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="203" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9211,7 +9208,7 @@
         <v>332</v>
       </c>
       <c r="E208" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F208" s="2" t="s">
         <v>332</v>
@@ -9243,7 +9240,7 @@
         <v>6</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E209" s="2" t="s">
         <v>189</v>
@@ -9264,7 +9261,7 @@
         <v>548</v>
       </c>
       <c r="K209" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="210" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9491,7 +9488,7 @@
         <v>332</v>
       </c>
       <c r="E216" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F216" s="2" t="s">
         <v>332</v>
@@ -9523,7 +9520,7 @@
         <v>10</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E217" s="2" t="s">
         <v>68</v>
@@ -9544,7 +9541,7 @@
         <v>616</v>
       </c>
       <c r="K217" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="218" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9736,7 +9733,7 @@
         <v>332</v>
       </c>
       <c r="E223" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F223" s="2" t="s">
         <v>332</v>
@@ -9768,7 +9765,7 @@
         <v>30</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E224" s="2" t="s">
         <v>177</v>
@@ -9783,13 +9780,13 @@
         <v>178</v>
       </c>
       <c r="I224" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J224" s="2">
         <v>860</v>
       </c>
       <c r="K224" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="225" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9806,7 +9803,7 @@
         <v>332</v>
       </c>
       <c r="E225" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F225" s="2">
         <v>30</v>
@@ -10086,7 +10083,7 @@
         <v>332</v>
       </c>
       <c r="E233" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F233" s="2" t="s">
         <v>332</v>
@@ -10118,7 +10115,7 @@
         <v>1</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E234" s="2" t="s">
         <v>154</v>
@@ -10133,13 +10130,13 @@
         <v>30</v>
       </c>
       <c r="I234" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J234" s="2">
         <v>256</v>
       </c>
       <c r="K234" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="235" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10191,7 +10188,7 @@
         <v>332</v>
       </c>
       <c r="E236" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F236" s="2" t="s">
         <v>332</v>
@@ -10223,7 +10220,7 @@
         <v>15</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E237" s="2" t="s">
         <v>129</v>
@@ -10238,13 +10235,13 @@
         <v>203</v>
       </c>
       <c r="I237" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J237" s="2">
         <v>590</v>
       </c>
       <c r="K237" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="238" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10436,7 +10433,7 @@
         <v>332</v>
       </c>
       <c r="E243" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F243" s="2" t="s">
         <v>332</v>
@@ -10468,7 +10465,7 @@
         <v>15</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E244" s="2" t="s">
         <v>68</v>
@@ -10483,13 +10480,13 @@
         <v>14</v>
       </c>
       <c r="I244" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J244" s="2">
         <v>605</v>
       </c>
       <c r="K244" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="245" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10681,7 +10678,7 @@
         <v>332</v>
       </c>
       <c r="E250" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F250" s="2" t="s">
         <v>332</v>
@@ -10713,7 +10710,7 @@
         <v>5</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E251" s="2" t="s">
         <v>10</v>
@@ -10728,13 +10725,13 @@
         <v>208</v>
       </c>
       <c r="I251" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J251" s="2">
         <v>570</v>
       </c>
       <c r="K251" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="252" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10856,7 +10853,7 @@
         <v>332</v>
       </c>
       <c r="E255" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F255" s="2" t="s">
         <v>332</v>
@@ -10888,7 +10885,7 @@
         <v>25</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E256" s="2" t="s">
         <v>210</v>
@@ -10903,13 +10900,13 @@
         <v>211</v>
       </c>
       <c r="I256" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J256" s="2">
         <v>857</v>
       </c>
       <c r="K256" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="257" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11171,7 +11168,7 @@
         <v>332</v>
       </c>
       <c r="E264" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F264" s="2" t="s">
         <v>332</v>
@@ -11203,7 +11200,7 @@
         <v>1</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E265" s="2" t="s">
         <v>209</v>
@@ -11218,13 +11215,13 @@
         <v>125</v>
       </c>
       <c r="I265" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J265" s="2">
         <v>306</v>
       </c>
       <c r="K265" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="266" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11241,7 +11238,7 @@
         <v>332</v>
       </c>
       <c r="E266" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F266" s="2">
         <v>40</v>
@@ -11276,7 +11273,7 @@
         <v>332</v>
       </c>
       <c r="E267" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F267" s="2" t="s">
         <v>332</v>
@@ -11308,7 +11305,7 @@
         <v>15</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E268" s="2" t="s">
         <v>115</v>
@@ -11323,13 +11320,13 @@
         <v>124</v>
       </c>
       <c r="I268" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J268" s="2">
         <v>551</v>
       </c>
       <c r="K268" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="269" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11521,7 +11518,7 @@
         <v>332</v>
       </c>
       <c r="E274" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F274" s="2" t="s">
         <v>332</v>
@@ -11553,7 +11550,7 @@
         <v>10</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E275" s="2" t="s">
         <v>133</v>
@@ -11568,13 +11565,13 @@
         <v>12</v>
       </c>
       <c r="I275" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J275" s="2">
         <v>610</v>
       </c>
       <c r="K275" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="276" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11731,7 +11728,7 @@
         <v>332</v>
       </c>
       <c r="E280" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F280" s="2" t="s">
         <v>332</v>
@@ -11763,7 +11760,7 @@
         <v>10</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E281" s="2" t="s">
         <v>180</v>
@@ -11778,13 +11775,13 @@
         <v>138</v>
       </c>
       <c r="I281" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J281" s="2">
         <v>579</v>
       </c>
       <c r="K281" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="282" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11836,7 +11833,7 @@
         <v>332</v>
       </c>
       <c r="E283" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F283" s="2">
         <v>60</v>
@@ -11906,7 +11903,7 @@
         <v>332</v>
       </c>
       <c r="E285" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F285" s="2" t="s">
         <v>332</v>
@@ -11938,7 +11935,7 @@
         <v>25</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E286" s="2" t="s">
         <v>228</v>
@@ -11953,13 +11950,13 @@
         <v>211</v>
       </c>
       <c r="I286" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J286" s="2">
         <v>853</v>
       </c>
       <c r="K286" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="287" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12011,7 +12008,7 @@
         <v>332</v>
       </c>
       <c r="E288" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F288" s="2">
         <v>122</v>
@@ -12256,7 +12253,7 @@
         <v>332</v>
       </c>
       <c r="E295" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F295" s="2" t="s">
         <v>332</v>
@@ -12288,7 +12285,7 @@
         <v>5</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E296" s="2" t="s">
         <v>189</v>
@@ -12303,13 +12300,13 @@
         <v>232</v>
       </c>
       <c r="I296" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J296" s="2">
         <v>584</v>
       </c>
       <c r="K296" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="297" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12501,7 +12498,7 @@
         <v>332</v>
       </c>
       <c r="E302" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F302" s="2" t="s">
         <v>332</v>
@@ -12533,7 +12530,7 @@
         <v>7</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E303" s="2" t="s">
         <v>193</v>
@@ -12548,13 +12545,13 @@
         <v>156</v>
       </c>
       <c r="I303" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J303" s="2">
         <v>567</v>
       </c>
       <c r="K303" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="304" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12746,7 +12743,7 @@
         <v>332</v>
       </c>
       <c r="E309" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F309" s="2" t="s">
         <v>332</v>
@@ -12778,7 +12775,7 @@
         <v>5</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E310" s="2" t="s">
         <v>223</v>
@@ -12793,13 +12790,13 @@
         <v>14</v>
       </c>
       <c r="I310" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J310" s="2">
         <v>551</v>
       </c>
       <c r="K310" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="311" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12956,7 +12953,7 @@
         <v>332</v>
       </c>
       <c r="E315" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F315" s="2" t="s">
         <v>332</v>
@@ -12988,7 +12985,7 @@
         <v>30</v>
       </c>
       <c r="D316" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E316" s="2" t="s">
         <v>72</v>
@@ -13003,13 +13000,13 @@
         <v>125</v>
       </c>
       <c r="I316" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J316" s="2">
         <v>829</v>
       </c>
       <c r="K316" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="317" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13306,7 +13303,7 @@
         <v>332</v>
       </c>
       <c r="E325" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F325" s="2" t="s">
         <v>332</v>
@@ -13338,10 +13335,10 @@
         <v>1</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E326" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F326" s="2">
         <v>60</v>
@@ -13359,7 +13356,7 @@
         <v>314</v>
       </c>
       <c r="K326" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="327" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13376,7 +13373,7 @@
         <v>332</v>
       </c>
       <c r="E327" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F327" s="2" t="s">
         <v>332</v>
@@ -13408,7 +13405,7 @@
         <v>10</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E328" s="2" t="s">
         <v>99</v>
@@ -13423,13 +13420,13 @@
         <v>127</v>
       </c>
       <c r="I328" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J328" s="2">
         <v>608</v>
       </c>
       <c r="K328" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="329" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13481,7 +13478,7 @@
         <v>332</v>
       </c>
       <c r="E330" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F330" s="2">
         <v>120</v>
@@ -13691,7 +13688,7 @@
         <v>332</v>
       </c>
       <c r="E336" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F336" s="2" t="s">
         <v>332</v>
@@ -13723,7 +13720,7 @@
         <v>30</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E337" s="2" t="s">
         <v>102</v>
@@ -13738,13 +13735,13 @@
         <v>238</v>
       </c>
       <c r="I337" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J337" s="2">
         <v>630</v>
       </c>
       <c r="K337" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="338" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13936,7 +13933,7 @@
         <v>332</v>
       </c>
       <c r="E343" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F343" s="2" t="s">
         <v>332</v>
@@ -13968,7 +13965,7 @@
         <v>5</v>
       </c>
       <c r="D344" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E344" s="2" t="s">
         <v>189</v>
@@ -13983,13 +13980,13 @@
         <v>126</v>
       </c>
       <c r="I344" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J344" s="2">
         <v>560</v>
       </c>
       <c r="K344" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="345" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -14181,7 +14178,7 @@
         <v>332</v>
       </c>
       <c r="E350" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F350" s="2" t="s">
         <v>332</v>
@@ -14213,7 +14210,7 @@
         <v>30</v>
       </c>
       <c r="D351" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E351" s="2" t="s">
         <v>103</v>
@@ -14228,13 +14225,13 @@
         <v>216</v>
       </c>
       <c r="I351" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J351" s="2">
         <v>876</v>
       </c>
       <c r="K351" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="352" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -14286,7 +14283,7 @@
         <v>332</v>
       </c>
       <c r="E353" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F353" s="2">
         <v>30</v>
@@ -14531,7 +14528,7 @@
         <v>332</v>
       </c>
       <c r="E360" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F360" s="2" t="s">
         <v>332</v>
@@ -14563,7 +14560,7 @@
         <v>1</v>
       </c>
       <c r="D361" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E361" s="2" t="s">
         <v>225</v>
@@ -14578,13 +14575,13 @@
         <v>226</v>
       </c>
       <c r="I361" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J361" s="2">
         <v>290</v>
       </c>
       <c r="K361" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="362" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -14636,7 +14633,7 @@
         <v>332</v>
       </c>
       <c r="E363" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F363" s="2" t="s">
         <v>332</v>
@@ -14668,7 +14665,7 @@
         <v>10</v>
       </c>
       <c r="D364" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E364" s="2" t="s">
         <v>99</v>
@@ -14683,13 +14680,13 @@
         <v>127</v>
       </c>
       <c r="I364" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J364" s="2">
         <v>594</v>
       </c>
       <c r="K364" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="365" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -14881,7 +14878,7 @@
         <v>332</v>
       </c>
       <c r="E370" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F370" s="2" t="s">
         <v>332</v>
@@ -14913,7 +14910,7 @@
         <v>10</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E371" s="2" t="s">
         <v>223</v>
@@ -14928,13 +14925,13 @@
         <v>208</v>
       </c>
       <c r="I371" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J371" s="2">
         <v>629</v>
       </c>
       <c r="K371" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="372" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -15091,7 +15088,7 @@
         <v>332</v>
       </c>
       <c r="E376" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F376" s="2" t="s">
         <v>332</v>
@@ -15123,7 +15120,7 @@
         <v>5</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E377" s="2" t="s">
         <v>189</v>
@@ -15138,13 +15135,13 @@
         <v>126</v>
       </c>
       <c r="I377" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J377" s="2">
         <v>618</v>
       </c>
       <c r="K377" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="378" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -15336,7 +15333,7 @@
         <v>332</v>
       </c>
       <c r="E383" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F383" s="2" t="s">
         <v>332</v>
@@ -15368,7 +15365,7 @@
         <v>30</v>
       </c>
       <c r="D384" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E384" s="2" t="s">
         <v>251</v>
@@ -15383,13 +15380,13 @@
         <v>178</v>
       </c>
       <c r="I384" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J384" s="2">
         <v>859</v>
       </c>
       <c r="K384" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="385" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -15511,7 +15508,7 @@
         <v>332</v>
       </c>
       <c r="E388" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F388" s="2">
         <v>3</v>
@@ -15651,7 +15648,7 @@
         <v>332</v>
       </c>
       <c r="E392" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F392" s="2" t="s">
         <v>332</v>
@@ -15683,7 +15680,7 @@
         <v>5</v>
       </c>
       <c r="D393" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E393" s="2" t="s">
         <v>236</v>
@@ -15698,13 +15695,13 @@
         <v>9</v>
       </c>
       <c r="I393" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J393" s="2">
         <v>279</v>
       </c>
       <c r="K393" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="394" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -15756,7 +15753,7 @@
         <v>332</v>
       </c>
       <c r="E395" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F395" s="2" t="s">
         <v>332</v>
@@ -15788,7 +15785,7 @@
         <v>15</v>
       </c>
       <c r="D396" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E396" s="2" t="s">
         <v>229</v>
@@ -15803,13 +15800,13 @@
         <v>257</v>
       </c>
       <c r="I396" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J396" s="2">
         <v>573</v>
       </c>
       <c r="K396" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="397" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -16083,7 +16080,7 @@
         <v>30</v>
       </c>
       <c r="I404" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J404" s="2" t="s">
         <v>332</v>
@@ -16106,7 +16103,7 @@
         <v>332</v>
       </c>
       <c r="E405" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F405" s="2" t="s">
         <v>332</v>
@@ -16138,7 +16135,7 @@
         <v>15</v>
       </c>
       <c r="D406" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E406" s="2" t="s">
         <v>189</v>
@@ -16153,13 +16150,13 @@
         <v>261</v>
       </c>
       <c r="I406" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J406" s="2">
         <v>624</v>
       </c>
       <c r="K406" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="407" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -16386,7 +16383,7 @@
         <v>332</v>
       </c>
       <c r="E413" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F413" s="2" t="s">
         <v>332</v>
@@ -16418,7 +16415,7 @@
         <v>5</v>
       </c>
       <c r="D414" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E414" s="2" t="s">
         <v>189</v>
@@ -16433,13 +16430,13 @@
         <v>126</v>
       </c>
       <c r="I414" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J414" s="2">
         <v>638</v>
       </c>
       <c r="K414" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="415" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -16631,7 +16628,7 @@
         <v>332</v>
       </c>
       <c r="E420" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F420" s="2" t="s">
         <v>332</v>
@@ -16663,7 +16660,7 @@
         <v>30</v>
       </c>
       <c r="D421" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E421" s="2" t="s">
         <v>102</v>
@@ -16678,13 +16675,13 @@
         <v>138</v>
       </c>
       <c r="I421" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J421" s="2">
         <v>908</v>
       </c>
       <c r="K421" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="422" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -16981,7 +16978,7 @@
         <v>332</v>
       </c>
       <c r="E430" s="2" t="s">
-        <v>333</v>
+        <v>499</v>
       </c>
       <c r="F430" s="2" t="s">
         <v>332</v>
@@ -17009,11 +17006,11 @@
       <c r="B431" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C431" s="2" t="s">
-        <v>332</v>
+      <c r="C431" s="2">
+        <v>1</v>
       </c>
       <c r="D431" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E431" s="2" t="s">
         <v>270</v>
@@ -17028,13 +17025,13 @@
         <v>226</v>
       </c>
       <c r="I431" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J431" s="2">
         <v>218</v>
       </c>
       <c r="K431" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="432" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -17086,7 +17083,7 @@
         <v>332</v>
       </c>
       <c r="E433" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F433" s="2" t="s">
         <v>332</v>
@@ -17118,7 +17115,7 @@
         <v>10</v>
       </c>
       <c r="D434" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E434" s="2" t="s">
         <v>189</v>
@@ -17133,13 +17130,13 @@
         <v>261</v>
       </c>
       <c r="I434" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J434" s="2">
         <v>572</v>
       </c>
       <c r="K434" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="435" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -17436,7 +17433,7 @@
         <v>332</v>
       </c>
       <c r="E443" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F443" s="2" t="s">
         <v>332</v>
@@ -17468,7 +17465,7 @@
         <v>10</v>
       </c>
       <c r="D444" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E444" s="2" t="s">
         <v>64</v>
@@ -17483,13 +17480,13 @@
         <v>130</v>
       </c>
       <c r="I444" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J444" s="2">
         <v>574</v>
       </c>
       <c r="K444" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="445" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -17646,7 +17643,7 @@
         <v>332</v>
       </c>
       <c r="E449" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F449" s="2" t="s">
         <v>332</v>
@@ -17678,7 +17675,7 @@
         <v>5</v>
       </c>
       <c r="D450" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E450" s="2" t="s">
         <v>133</v>
@@ -17693,13 +17690,13 @@
         <v>278</v>
       </c>
       <c r="I450" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J450" s="2">
         <v>554</v>
       </c>
       <c r="K450" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="451" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -17786,7 +17783,7 @@
         <v>332</v>
       </c>
       <c r="E453" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F453" s="2" t="s">
         <v>332</v>
@@ -17818,7 +17815,7 @@
         <v>25</v>
       </c>
       <c r="D454" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E454" s="2" t="s">
         <v>267</v>
@@ -17833,13 +17830,13 @@
         <v>178</v>
       </c>
       <c r="I454" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J454" s="2">
         <v>890</v>
       </c>
       <c r="K454" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="455" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -18101,7 +18098,7 @@
         <v>332</v>
       </c>
       <c r="E462" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F462" s="2" t="s">
         <v>332</v>
@@ -18129,11 +18126,11 @@
       <c r="B463" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C463" s="2" t="s">
-        <v>332</v>
+      <c r="C463" s="2">
+        <v>1</v>
       </c>
       <c r="D463" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E463" s="2" t="s">
         <v>92</v>
@@ -18148,13 +18145,13 @@
         <v>30</v>
       </c>
       <c r="I463" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J463" s="2">
         <v>288</v>
       </c>
       <c r="K463" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="464" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -18206,7 +18203,7 @@
         <v>332</v>
       </c>
       <c r="E465" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F465" s="2" t="s">
         <v>332</v>
@@ -18238,7 +18235,7 @@
         <v>25</v>
       </c>
       <c r="D466" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E466" s="2" t="s">
         <v>175</v>
@@ -18253,13 +18250,13 @@
         <v>6</v>
       </c>
       <c r="I466" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J466" s="2">
         <v>616</v>
       </c>
       <c r="K466" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="467" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -18416,7 +18413,7 @@
         <v>332</v>
       </c>
       <c r="E471" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F471" s="2">
         <v>30</v>
@@ -18451,7 +18448,7 @@
         <v>332</v>
       </c>
       <c r="E472" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F472" s="2" t="s">
         <v>332</v>
@@ -18483,7 +18480,7 @@
         <v>10</v>
       </c>
       <c r="D473" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E473" s="2" t="s">
         <v>189</v>
@@ -18498,13 +18495,13 @@
         <v>289</v>
       </c>
       <c r="I473" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J473" s="2">
         <v>596</v>
       </c>
       <c r="K473" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="474" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -18731,7 +18728,7 @@
         <v>332</v>
       </c>
       <c r="E480" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F480" s="2" t="s">
         <v>332</v>
@@ -18763,7 +18760,7 @@
         <v>5</v>
       </c>
       <c r="D481" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E481" s="2" t="s">
         <v>64</v>
@@ -18778,13 +18775,13 @@
         <v>130</v>
       </c>
       <c r="I481" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J481" s="2">
         <v>581</v>
       </c>
       <c r="K481" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="482" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -18941,7 +18938,7 @@
         <v>332</v>
       </c>
       <c r="E486" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F486" s="2" t="s">
         <v>332</v>
@@ -18973,7 +18970,7 @@
         <v>30</v>
       </c>
       <c r="D487" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E487" s="2" t="s">
         <v>220</v>
@@ -18988,13 +18985,13 @@
         <v>12</v>
       </c>
       <c r="I487" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="J487" s="2">
         <v>852</v>
       </c>
       <c r="K487" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="488" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -19361,7 +19358,7 @@
         <v>332</v>
       </c>
       <c r="E498" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F498" s="2" t="s">
         <v>332</v>
@@ -19393,7 +19390,7 @@
         <v>1</v>
       </c>
       <c r="D499" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E499" s="2" t="s">
         <v>131</v>
@@ -19408,13 +19405,13 @@
         <v>268</v>
       </c>
       <c r="I499" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J499" s="2">
         <v>284</v>
       </c>
       <c r="K499" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="500" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -19431,7 +19428,7 @@
         <v>332</v>
       </c>
       <c r="E500" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F500" s="2">
         <v>40</v>
@@ -19466,7 +19463,7 @@
         <v>332</v>
       </c>
       <c r="E501" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F501" s="2" t="s">
         <v>332</v>
@@ -19498,7 +19495,7 @@
         <v>15</v>
       </c>
       <c r="D502" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E502" s="2" t="s">
         <v>189</v>
@@ -19513,13 +19510,13 @@
         <v>289</v>
       </c>
       <c r="I502" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J502" s="2">
         <v>614</v>
       </c>
       <c r="K502" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="503" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -19816,7 +19813,7 @@
         <v>332</v>
       </c>
       <c r="E511" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F511" s="2" t="s">
         <v>332</v>
@@ -19848,7 +19845,7 @@
         <v>15</v>
       </c>
       <c r="D512" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E512" s="2" t="s">
         <v>92</v>
@@ -19863,13 +19860,13 @@
         <v>30</v>
       </c>
       <c r="I512" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J512" s="2">
         <v>630</v>
       </c>
       <c r="K512" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="513" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -20026,7 +20023,7 @@
         <v>332</v>
       </c>
       <c r="E517" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F517" s="2" t="s">
         <v>332</v>
@@ -20058,7 +20055,7 @@
         <v>5</v>
       </c>
       <c r="D518" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E518" s="2" t="s">
         <v>189</v>
@@ -20073,13 +20070,13 @@
         <v>126</v>
       </c>
       <c r="I518" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J518" s="2">
         <v>561</v>
       </c>
       <c r="K518" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="519" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -20306,7 +20303,7 @@
         <v>332</v>
       </c>
       <c r="E525" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F525" s="2" t="s">
         <v>332</v>
@@ -20338,7 +20335,7 @@
         <v>25</v>
       </c>
       <c r="D526" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E526" s="2" t="s">
         <v>332</v>
@@ -20353,13 +20350,13 @@
         <v>303</v>
       </c>
       <c r="I526" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="J526" s="2">
         <v>895</v>
       </c>
       <c r="K526" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="527" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -20621,7 +20618,7 @@
         <v>332</v>
       </c>
       <c r="E534" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F534" s="2" t="s">
         <v>332</v>
@@ -20653,7 +20650,7 @@
         <v>5</v>
       </c>
       <c r="D535" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E535" s="2" t="s">
         <v>271</v>
@@ -20668,13 +20665,13 @@
         <v>138</v>
       </c>
       <c r="I535" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J535" s="2">
         <v>289</v>
       </c>
       <c r="K535" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="536" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -20761,7 +20758,7 @@
         <v>332</v>
       </c>
       <c r="E538" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F538" s="2" t="s">
         <v>332</v>
@@ -20793,7 +20790,7 @@
         <v>12</v>
       </c>
       <c r="D539" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E539" s="2" t="s">
         <v>193</v>
@@ -20808,13 +20805,13 @@
         <v>307</v>
       </c>
       <c r="I539" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="J539" s="2">
         <v>565</v>
       </c>
       <c r="K539" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="540" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -20948,7 +20945,7 @@
         <v>127</v>
       </c>
       <c r="I543" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J543" s="2" t="s">
         <v>332</v>
@@ -21041,7 +21038,7 @@
         <v>332</v>
       </c>
       <c r="E546" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F546" s="2" t="s">
         <v>332</v>
@@ -21073,7 +21070,7 @@
         <v>20</v>
       </c>
       <c r="D547" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E547" s="2" t="s">
         <v>310</v>
@@ -21088,13 +21085,13 @@
         <v>126</v>
       </c>
       <c r="I547" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J547" s="2">
         <v>581</v>
       </c>
       <c r="K547" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="548" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -21286,7 +21283,7 @@
         <v>332</v>
       </c>
       <c r="E553" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F553" s="2" t="s">
         <v>332</v>
@@ -21318,7 +21315,7 @@
         <v>5</v>
       </c>
       <c r="D554" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E554" s="2" t="s">
         <v>96</v>
@@ -21333,13 +21330,13 @@
         <v>6</v>
       </c>
       <c r="I554" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J554" s="2">
         <v>617</v>
       </c>
       <c r="K554" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="555" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -21496,7 +21493,7 @@
         <v>332</v>
       </c>
       <c r="E559" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F559" s="2" t="s">
         <v>332</v>
@@ -21528,7 +21525,7 @@
         <v>30</v>
       </c>
       <c r="D560" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E560" s="2" t="s">
         <v>210</v>
@@ -21543,13 +21540,13 @@
         <v>178</v>
       </c>
       <c r="I560" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J560" s="2">
         <v>882</v>
       </c>
       <c r="K560" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="561" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -21881,7 +21878,7 @@
         <v>332</v>
       </c>
       <c r="E570" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F570" s="2" t="s">
         <v>332</v>
@@ -21909,14 +21906,14 @@
       <c r="B571" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C571" s="2" t="s">
-        <v>332</v>
+      <c r="C571" s="2">
+        <v>1</v>
       </c>
       <c r="D571" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E571" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F571" s="2">
         <v>60</v>
@@ -21928,13 +21925,13 @@
         <v>244</v>
       </c>
       <c r="I571" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J571" s="2">
         <v>314</v>
       </c>
       <c r="K571" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="572" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -21951,7 +21948,7 @@
         <v>332</v>
       </c>
       <c r="E572" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F572" s="2" t="s">
         <v>332</v>
@@ -21983,7 +21980,7 @@
         <v>10</v>
       </c>
       <c r="D573" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E573" s="2" t="s">
         <v>301</v>
@@ -21998,7 +21995,7 @@
         <v>126</v>
       </c>
       <c r="I573" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J573" s="2">
         <v>596</v>
@@ -22161,7 +22158,7 @@
         <v>332</v>
       </c>
       <c r="E578" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F578" s="2" t="s">
         <v>332</v>
@@ -22193,7 +22190,7 @@
         <v>30</v>
       </c>
       <c r="D579" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E579" s="2" t="s">
         <v>317</v>
@@ -22208,13 +22205,13 @@
         <v>320</v>
       </c>
       <c r="I579" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J579" s="2">
         <v>636</v>
       </c>
       <c r="K579" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="580" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -22441,7 +22438,7 @@
         <v>332</v>
       </c>
       <c r="E586" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F586" s="2" t="s">
         <v>332</v>
@@ -22473,7 +22470,7 @@
         <v>5</v>
       </c>
       <c r="D587" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E587" s="2" t="s">
         <v>202</v>
@@ -22488,13 +22485,13 @@
         <v>12</v>
       </c>
       <c r="I587" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J587" s="2">
         <v>603</v>
       </c>
       <c r="K587" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="588" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -22651,7 +22648,7 @@
         <v>332</v>
       </c>
       <c r="E592" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F592" s="2" t="s">
         <v>332</v>
@@ -22683,7 +22680,7 @@
         <v>30</v>
       </c>
       <c r="D593" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E593" s="2" t="s">
         <v>323</v>
@@ -22698,13 +22695,13 @@
         <v>326</v>
       </c>
       <c r="I593" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J593" s="2">
         <v>814</v>
       </c>
       <c r="K593" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="594" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -23001,7 +22998,7 @@
         <v>332</v>
       </c>
       <c r="E602" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F602" s="2" t="s">
         <v>332</v>
@@ -23033,7 +23030,7 @@
         <v>5</v>
       </c>
       <c r="D603" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E603" s="2" t="s">
         <v>170</v>
@@ -23048,13 +23045,13 @@
         <v>208</v>
       </c>
       <c r="I603" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J603" s="2">
         <v>304</v>
       </c>
       <c r="K603" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="604" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -23106,7 +23103,7 @@
         <v>332</v>
       </c>
       <c r="E605" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F605" s="2" t="s">
         <v>332</v>
@@ -23138,7 +23135,7 @@
         <v>15</v>
       </c>
       <c r="D606" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E606" s="2" t="s">
         <v>64</v>
@@ -23153,13 +23150,13 @@
         <v>329</v>
       </c>
       <c r="I606" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="J606" s="2">
         <v>599</v>
       </c>
       <c r="K606" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="607" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -23456,7 +23453,7 @@
         <v>332</v>
       </c>
       <c r="E615" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F615" s="2" t="s">
         <v>332</v>

</xml_diff>